<commit_message>
Timeline - Added disclosureType in response.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/APIList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/APIList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nohr/OneDrive/Skrum/07_プロダクト開発/プロダクト資料/01_要件定義/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nohr/Dev/skrum/skrum_docs/02_SpecificationDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="更新履歴" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="405">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -2080,20 +2080,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>追加ユーザ検索</t>
-    <rPh sb="0" eb="2">
-      <t>ツイk</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ケンサk</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>/api/additionalusers/search.json</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>searchAdditionalusersAction()</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2125,6 +2111,24 @@
   </si>
   <si>
     <t>AH0211</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AH0106</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>追加グループメンバー検索</t>
+    <rPh sb="0" eb="2">
+      <t>ツイk</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ケンサk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/additionalusers/search.json</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5751,8 +5755,8 @@
         <v>21</v>
       </c>
       <c r="F46" s="5">
-        <f>F44+1</f>
-        <v>4</v>
+        <f>F45+1</f>
+        <v>5</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>84</v>
@@ -5802,7 +5806,7 @@
       </c>
       <c r="F47" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>336</v>
@@ -6016,11 +6020,11 @@
         <v>259</v>
       </c>
       <c r="K51" s="39" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L51" s="39"/>
       <c r="M51" s="39" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="N51" s="32" t="s">
         <v>288</v>
@@ -6136,14 +6140,14 @@
         <v>50</v>
       </c>
       <c r="B54" s="17">
-        <f t="shared" si="3"/>
+        <f>IF(C54=C58,B58,B58+1)</f>
         <v>8</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>283</v>
+        <v>81</v>
       </c>
       <c r="D54" s="17">
-        <f t="shared" si="2"/>
+        <f>IF(B54=B58,IF(E54=E58,D58,D58+1),1)</f>
         <v>2</v>
       </c>
       <c r="E54" s="17" t="s">
@@ -6157,122 +6161,125 @@
         <v>42</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>143</v>
+        <v>252</v>
       </c>
       <c r="J54" s="17" t="s">
-        <v>94</v>
+        <v>259</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="L54" s="17"/>
       <c r="M54" s="17" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="N54" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="O54" s="18"/>
+        <v>288</v>
+      </c>
+      <c r="O54" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="P54" s="42"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="17">
+      <c r="A55" s="39">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B55" s="17">
-        <f t="shared" si="3"/>
+      <c r="B55" s="5">
+        <f t="shared" ref="B55" si="14">IF(C55=C54,B54,B54+1)</f>
         <v>8</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C55" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="D55" s="17">
-        <f t="shared" si="2"/>
+      <c r="D55" s="5">
+        <f t="shared" ref="D55" si="15">IF(B55=B54,IF(E55=E54,D54,D54+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F55" s="17">
+      <c r="F55" s="5">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="G55" s="17" t="s">
-        <v>338</v>
-      </c>
-      <c r="H55" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I55" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="J55" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K55" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="N55" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="O55" s="18"/>
+      <c r="G55" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="L55" s="6"/>
+      <c r="M55" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="N55" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="O55" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P55" s="42"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="5">
+      <c r="A56" s="17">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B56" s="5">
-        <f t="shared" si="3"/>
+      <c r="B56" s="17">
+        <f>IF(C56=C53,B53,B53+1)</f>
         <v>8</v>
       </c>
-      <c r="C56" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="5">
-        <f t="shared" si="2"/>
+      <c r="C56" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="D56" s="17">
+        <f>IF(B56=B53,IF(E56=E53,D53,D53+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F56" s="39">
+      <c r="E56" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F56" s="17">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="G56" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="K56" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L56" s="6"/>
-      <c r="M56" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="N56" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="O56" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P56" s="42"/>
+      <c r="G56" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H56" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J56" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="K56" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="O56" s="18"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="17">
@@ -6284,7 +6291,7 @@
         <v>8</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>81</v>
+        <v>283</v>
       </c>
       <c r="D57" s="17">
         <f t="shared" si="2"/>
@@ -6298,76 +6305,73 @@
         <v>10</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="I57" s="17" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="J57" s="17" t="s">
-        <v>259</v>
+        <v>112</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>116</v>
+        <v>181</v>
       </c>
       <c r="L57" s="17"/>
       <c r="M57" s="17" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="N57" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="O57" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="P57" s="42"/>
+        <v>260</v>
+      </c>
+      <c r="O57" s="18"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="39">
+      <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B58" s="5">
-        <f t="shared" ref="B58" si="14">IF(C58=C57,B57,B57+1)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C58" s="39" t="s">
-        <v>283</v>
+      <c r="C58" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="D58" s="5">
-        <f t="shared" ref="D58" si="15">IF(B58=B57,IF(E58=E57,D57,D57+1),1)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E58" s="39" t="s">
-        <v>66</v>
+      <c r="E58" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="F58" s="5">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G58" s="39" t="s">
-        <v>282</v>
+      <c r="G58" s="5" t="s">
+        <v>339</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>395</v>
+        <v>43</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>390</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>396</v>
+        <v>113</v>
       </c>
       <c r="L58" s="6"/>
       <c r="M58" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="N58" s="32" t="s">
-        <v>288</v>
+        <v>211</v>
+      </c>
+      <c r="N58" s="29" t="s">
+        <v>234</v>
       </c>
       <c r="O58" s="37" t="s">
         <v>12</v>
@@ -6380,14 +6384,14 @@
         <v>55</v>
       </c>
       <c r="B59" s="5">
-        <f t="shared" ref="B59" si="16">IF(C59=C58,B58,B58+1)</f>
+        <f>IF(C59=C55,B55,B55+1)</f>
         <v>8</v>
       </c>
       <c r="C59" s="39" t="s">
         <v>283</v>
       </c>
       <c r="D59" s="5">
-        <f t="shared" ref="D59" si="17">IF(B59=B58,IF(E59=E58,D58,D58+1),1)</f>
+        <f>IF(B59=B55,IF(E59=E55,D55,D55+1),1)</f>
         <v>2</v>
       </c>
       <c r="E59" s="39" t="s">
@@ -6401,7 +6405,7 @@
         <v>282</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>391</v>
@@ -6410,11 +6414,11 @@
         <v>60</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L59" s="6"/>
       <c r="M59" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="N59" s="32" t="s">
         <v>288</v>
@@ -6430,14 +6434,14 @@
         <v>56</v>
       </c>
       <c r="B60" s="5">
-        <f>IF(C60=C57,B57,B57+1)</f>
+        <f>IF(C60=C54,B54,B54+1)</f>
         <v>8</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>81</v>
       </c>
       <c r="D60" s="5">
-        <f>IF(B60=B57,IF(E60=E57,D57,D57+1),1)</f>
+        <f>IF(B60=B54,IF(E60=E54,D54,D54+1),1)</f>
         <v>2</v>
       </c>
       <c r="E60" s="5" t="s">
@@ -6454,7 +6458,7 @@
         <v>282</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J60" s="5" t="s">
         <v>284</v>
@@ -6830,14 +6834,14 @@
         <v>64</v>
       </c>
       <c r="B68" s="5">
-        <f t="shared" ref="B68" si="18">IF(C68=C67,B67,B67+1)</f>
+        <f t="shared" ref="B68" si="16">IF(C68=C67,B67,B67+1)</f>
         <v>11</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D68" s="5">
-        <f t="shared" ref="D68" si="19">IF(B68=B67,IF(E68=E67,D67,D67+1),1)</f>
+        <f t="shared" ref="D68" si="17">IF(B68=B67,IF(E68=E67,D67,D67+1),1)</f>
         <v>1</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -6882,14 +6886,14 @@
         <v>65</v>
       </c>
       <c r="B69" s="5">
-        <f t="shared" ref="B69" si="20">IF(C69=C68,B68,B68+1)</f>
+        <f t="shared" ref="B69" si="18">IF(C69=C68,B68,B68+1)</f>
         <v>11</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D69" s="5">
-        <f t="shared" ref="D69" si="21">IF(B69=B68,IF(E69=E68,D68,D68+1),1)</f>
+        <f t="shared" ref="D69" si="19">IF(B69=B68,IF(E69=E68,D68,D68+1),1)</f>
         <v>1</v>
       </c>
       <c r="E69" s="5" t="s">
@@ -7080,14 +7084,14 @@
         <v>69</v>
       </c>
       <c r="B73" s="17">
-        <f t="shared" ref="B73" si="22">IF(C73=C72,B72,B72+1)</f>
+        <f t="shared" ref="B73" si="20">IF(C73=C72,B72,B72+1)</f>
         <v>11</v>
       </c>
       <c r="C73" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D73" s="17">
-        <f t="shared" ref="D73" si="23">IF(B73=B72,IF(E73=E72,D72,D72+1),1)</f>
+        <f t="shared" ref="D73" si="21">IF(B73=B72,IF(E73=E72,D72,D72+1),1)</f>
         <v>2</v>
       </c>
       <c r="E73" s="17" t="s">
@@ -7225,7 +7229,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
-        <f t="shared" ref="A76:A82" si="24">ROW()-4</f>
+        <f t="shared" ref="A76:A82" si="22">ROW()-4</f>
         <v>72</v>
       </c>
       <c r="B76" s="5">
@@ -7243,7 +7247,7 @@
         <v>26</v>
       </c>
       <c r="F76" s="5">
-        <f t="shared" ref="F76:F79" si="25">F75+1</f>
+        <f t="shared" ref="F76:F79" si="23">F75+1</f>
         <v>2</v>
       </c>
       <c r="G76" s="5" t="s">
@@ -7277,7 +7281,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>73</v>
       </c>
       <c r="B77" s="5">
@@ -7295,7 +7299,7 @@
         <v>26</v>
       </c>
       <c r="F77" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>3</v>
       </c>
       <c r="G77" s="5" t="s">
@@ -7329,7 +7333,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>74</v>
       </c>
       <c r="B78" s="5">
@@ -7347,7 +7351,7 @@
         <v>26</v>
       </c>
       <c r="F78" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>4</v>
       </c>
       <c r="G78" s="5" t="s">
@@ -7381,7 +7385,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>75</v>
       </c>
       <c r="B79" s="5">
@@ -7399,7 +7403,7 @@
         <v>26</v>
       </c>
       <c r="F79" s="5">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="G79" s="5" t="s">
@@ -7433,7 +7437,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>76</v>
       </c>
       <c r="B80" s="5">
@@ -7484,7 +7488,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>77</v>
       </c>
       <c r="B81" s="5">
@@ -7535,7 +7539,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>78</v>
       </c>
       <c r="B82" s="5">

</xml_diff>

<commit_message>
Timeline - Added deleting a post.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/APIList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/APIList.xlsx
@@ -16,7 +16,7 @@
     <sheet name="API一覧" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">API一覧!$A$4:$N$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">API一覧!$A$4:$N$84</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="413">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -2129,6 +2129,53 @@
   </si>
   <si>
     <t>/api/additionalusers/search.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿削除</t>
+    <rPh sb="0" eb="2">
+      <t>トウコ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>サk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿公開設定変更</t>
+    <rPh sb="0" eb="2">
+      <t>トウコ</t>
+    </rPh>
+    <rPh sb="2" eb="6">
+      <t>コウカ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ヘンコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AG0404</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/posts/{slug}.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deletePostAction($slug)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/posts/{slug}/changedisclosure.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>changePostDisclosureAction($slug)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AG0405</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3583,7 +3630,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q118"/>
+  <dimension ref="A1:Q120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3710,7 +3757,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <f t="shared" ref="A5:A75" si="0">ROW()-4</f>
+        <f t="shared" ref="A5:A77" si="0">ROW()-4</f>
         <v>1</v>
       </c>
       <c r="B5" s="5">
@@ -3917,7 +3964,7 @@
         <v>90</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ref="D9:D82" si="2">IF(B9=B8,IF(E9=E8,D8,D8+1),1)</f>
+        <f t="shared" ref="D9:D84" si="2">IF(B9=B8,IF(E9=E8,D8,D8+1),1)</f>
         <v>1</v>
       </c>
       <c r="E9" s="16" t="s">
@@ -3959,7 +4006,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="5">
-        <f t="shared" ref="B10:B82" si="3">IF(C10=C9,B9,B9+1)</f>
+        <f t="shared" ref="B10:B84" si="3">IF(C10=C9,B9,B9+1)</f>
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -3973,7 +4020,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" ref="F10:F73" si="5">F9+1</f>
+        <f t="shared" ref="F10:F75" si="5">F9+1</f>
         <v>2</v>
       </c>
       <c r="G10" s="16" t="s">
@@ -5542,43 +5589,44 @@
         <v>38</v>
       </c>
       <c r="B42" s="5">
-        <f>IF(C42=C40,B40,B40+1)</f>
-        <v>8</v>
+        <f t="shared" ref="B42" si="12">IF(C42=C41,B41,B41+1)</f>
+        <v>7</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="D42" s="5">
-        <f>IF(B42=B40,IF(E42=E40,D40,D40+1),1)</f>
-        <v>1</v>
+        <f t="shared" ref="D42" si="13">IF(B42=B40,IF(E42=E40,D40,D40+1),1)</f>
+        <v>3</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>21</v>
+        <v>367</v>
       </c>
       <c r="F42" s="5">
-        <v>1</v>
+        <f>F41+1</f>
+        <v>4</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>86</v>
+        <v>405</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>141</v>
+        <v>407</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>109</v>
+        <v>408</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="N42" s="29" t="s">
-        <v>255</v>
+        <v>409</v>
+      </c>
+      <c r="N42" s="27" t="s">
+        <v>235</v>
       </c>
       <c r="O42" s="37" t="s">
         <v>12</v>
@@ -5591,144 +5639,143 @@
         <v>39</v>
       </c>
       <c r="B43" s="5">
+        <f t="shared" ref="B43" si="14">IF(C43=C42,B42,B42+1)</f>
+        <v>7</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" ref="D43" si="15">IF(B43=B41,IF(E43=E41,D41,D41+1),1)</f>
+        <v>3</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="F43" s="5">
+        <f>F42+1</f>
+        <v>5</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="L43" s="6"/>
+      <c r="M43" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="N43" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="O43" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P43" s="42"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B44" s="5">
+        <f>IF(C44=C40,B40,B40+1)</f>
+        <v>8</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="5">
+        <f>IF(B44=B40,IF(E44=E40,D40,D40+1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L44" s="6"/>
+      <c r="M44" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="N44" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="O44" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P44" s="42"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B45" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C45" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D45" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F45" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G43" s="16" t="s">
+      <c r="G45" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I45" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="J45" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="K45" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="L43" s="6"/>
-      <c r="M43" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="N43" s="45" t="s">
-        <v>233</v>
-      </c>
-      <c r="O43" s="37" t="s">
-        <v>278</v>
-      </c>
-      <c r="P43" s="42"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="17">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B44" s="17">
-        <f>IF(C44=C43,B43,B43+1)</f>
-        <v>8</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="D44" s="17">
-        <f>IF(B44=B43,IF(E44=E43,D43,D43+1),1)</f>
-        <v>1</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F44" s="17">
-        <f>F43+1</f>
-        <v>3</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>300</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="N44" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="O44" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="P44" s="42"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B45" s="5">
-        <f>IF(C45=C44,B44,B44+1)</f>
-        <v>8</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="5">
-        <f>IF(B45=B44,IF(E45=E44,D44,D44+1),1)</f>
-        <v>1</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="5">
-        <f>F44+1</f>
-        <v>4</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>393</v>
       </c>
       <c r="L45" s="6"/>
       <c r="M45" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="N45" s="32" t="s">
-        <v>288</v>
+        <v>206</v>
+      </c>
+      <c r="N45" s="45" t="s">
+        <v>233</v>
       </c>
       <c r="O45" s="37" t="s">
         <v>278</v>
@@ -5736,52 +5783,52 @@
       <c r="P45" s="42"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+      <c r="A46" s="17">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B46" s="5">
-        <f>IF(C46=C44,B44,B44+1)</f>
+      <c r="B46" s="17">
+        <f>IF(C46=C45,B45,B45+1)</f>
         <v>8</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="5">
-        <f>IF(B46=B44,IF(E46=E44,D44,D44+1),1)</f>
+      <c r="C46" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="D46" s="17">
+        <f>IF(B46=B45,IF(E46=E45,D45,D45+1),1)</f>
         <v>1</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46" s="5">
+      <c r="E46" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F46" s="17">
         <f>F45+1</f>
-        <v>5</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L46" s="6"/>
-      <c r="M46" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="N46" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="O46" s="37" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="J46" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="N46" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="O46" s="18" t="s">
+        <v>278</v>
       </c>
       <c r="P46" s="42"/>
     </row>
@@ -5791,44 +5838,44 @@
         <v>43</v>
       </c>
       <c r="B47" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C47=C46,B46,B46+1)</f>
         <v>8</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>81</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(B47=B46,IF(E47=E46,D46,D46+1),1)</f>
         <v>1</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F47" s="5">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f>F46+1</f>
+        <v>4</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>336</v>
+        <v>83</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>87</v>
+        <v>392</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>385</v>
+        <v>143</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>181</v>
+        <v>393</v>
       </c>
       <c r="L47" s="6"/>
       <c r="M47" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="N47" s="28" t="s">
-        <v>237</v>
+        <v>394</v>
+      </c>
+      <c r="N47" s="32" t="s">
+        <v>288</v>
       </c>
       <c r="O47" s="37" t="s">
         <v>278</v>
@@ -5841,40 +5888,41 @@
         <v>44</v>
       </c>
       <c r="B48" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C48=C46,B46,B46+1)</f>
         <v>8</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>81</v>
       </c>
       <c r="D48" s="5">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>IF(B48=B46,IF(E48=E46,D46,D46+1),1)</f>
+        <v>1</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F48" s="5">
-        <v>1</v>
-      </c>
-      <c r="G48" s="16" t="s">
+        <f>F47+1</f>
         <v>5</v>
       </c>
+      <c r="G48" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="H48" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="K48" s="6" t="s">
         <v>111</v>
       </c>
       <c r="L48" s="6"/>
       <c r="M48" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N48" s="28" t="s">
         <v>237</v>
@@ -5898,749 +5946,749 @@
       </c>
       <c r="D49" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F49" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>336</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>146</v>
+        <v>385</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>113</v>
+        <v>181</v>
       </c>
       <c r="L49" s="6"/>
       <c r="M49" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="N49" s="29" t="s">
-        <v>234</v>
+        <v>226</v>
+      </c>
+      <c r="N49" s="28" t="s">
+        <v>237</v>
       </c>
       <c r="O49" s="37" t="s">
-        <v>12</v>
+        <v>278</v>
       </c>
       <c r="P49" s="42"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" s="17">
+      <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B50" s="17">
+      <c r="B50" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L50" s="6"/>
+      <c r="M50" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="N50" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="O50" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P50" s="42"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B51" s="5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L51" s="6"/>
+      <c r="M51" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="N51" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="O51" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P51" s="42"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52" s="17">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B52" s="17">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E52" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F50" s="17">
+      <c r="F52" s="17">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="G52" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H50" s="17" t="s">
+      <c r="H52" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="I50" s="17" t="s">
+      <c r="I52" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J52" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="K50" s="17" t="s">
+      <c r="K52" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17" t="s">
+      <c r="L52" s="17"/>
+      <c r="M52" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="N50" s="17" t="s">
+      <c r="N52" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="O50" s="18" t="s">
+      <c r="O52" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P50" s="42"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="39">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B51" s="5">
-        <f t="shared" ref="B51" si="12">IF(C51=C50,B50,B50+1)</f>
+      <c r="P52" s="42"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53" s="39">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B53" s="5">
+        <f t="shared" ref="B53" si="16">IF(C53=C52,B52,B52+1)</f>
         <v>8</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C53" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="5">
-        <f t="shared" ref="D51" si="13">IF(B51=B50,IF(E51=E50,D50,D50+1),1)</f>
+      <c r="D53" s="5">
+        <f t="shared" ref="D53" si="17">IF(B53=B52,IF(E53=E52,D52,D52+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E51" s="39" t="s">
+      <c r="E53" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F53" s="5">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="G51" s="39" t="s">
+      <c r="G53" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H51" s="39" t="s">
+      <c r="H53" s="39" t="s">
         <v>387</v>
       </c>
-      <c r="I51" s="39" t="s">
+      <c r="I53" s="39" t="s">
         <v>388</v>
       </c>
-      <c r="J51" s="39" t="s">
+      <c r="J53" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="K51" s="39" t="s">
+      <c r="K53" s="39" t="s">
         <v>396</v>
       </c>
-      <c r="L51" s="39"/>
-      <c r="M51" s="39" t="s">
+      <c r="L53" s="39"/>
+      <c r="M53" s="39" t="s">
         <v>397</v>
       </c>
-      <c r="N51" s="32" t="s">
+      <c r="N53" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="O51" s="37" t="s">
+      <c r="O53" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P51" s="42"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A52" s="5">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B52" s="5">
-        <f>IF(C52=C50,B50,B50+1)</f>
+      <c r="P53" s="42"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B54" s="5">
+        <f>IF(C54=C52,B52,B52+1)</f>
         <v>8</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C54" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D52" s="5">
-        <f>IF(B52=B50,IF(E52=E50,D50,D50+1),1)</f>
+      <c r="D54" s="5">
+        <f>IF(B54=B52,IF(E54=E52,D52,D52+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F54" s="5">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="G52" s="5" t="s">
+      <c r="G54" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="H54" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="I54" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J52" s="5" t="s">
+      <c r="J54" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K52" s="6" t="s">
+      <c r="K54" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="L52" s="6"/>
-      <c r="M52" s="5" t="s">
+      <c r="L54" s="6"/>
+      <c r="M54" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="N52" s="30" t="s">
+      <c r="N54" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="O52" s="37" t="s">
+      <c r="O54" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P52" s="42"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A53" s="5">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B53" s="5">
+      <c r="P54" s="42"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55" s="5">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B55" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D55" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F55" s="5">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="G53" s="5" t="s">
+      <c r="G55" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H55" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="I53" s="5" t="s">
+      <c r="I55" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="J53" s="5" t="s">
+      <c r="J55" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="K53" s="6" t="s">
+      <c r="K55" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="L53" s="6"/>
-      <c r="M53" s="5" t="s">
+      <c r="L55" s="6"/>
+      <c r="M55" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="N53" s="30" t="s">
+      <c r="N55" s="30" t="s">
         <v>287</v>
       </c>
-      <c r="O53" s="37" t="s">
+      <c r="O55" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P53" s="42"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A54" s="17">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B54" s="17">
-        <f>IF(C54=C58,B58,B58+1)</f>
+      <c r="P55" s="42"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56" s="17">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B56" s="17">
+        <f>IF(C56=C60,B60,B60+1)</f>
         <v>8</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C56" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="17">
-        <f>IF(B54=B58,IF(E54=E58,D58,D58+1),1)</f>
+      <c r="D56" s="17">
+        <f>IF(B56=B60,IF(E56=E60,D60,D60+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E56" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F54" s="17">
+      <c r="F56" s="17">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="G56" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H54" s="17" t="s">
+      <c r="H56" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I56" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="J54" s="17" t="s">
+      <c r="J56" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="K54" s="17" t="s">
+      <c r="K56" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17" t="s">
+      <c r="L56" s="17"/>
+      <c r="M56" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="N54" s="17" t="s">
+      <c r="N56" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="O54" s="18" t="s">
+      <c r="O56" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P54" s="42"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A55" s="39">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B55" s="5">
-        <f t="shared" ref="B55" si="14">IF(C55=C54,B54,B54+1)</f>
+      <c r="P56" s="42"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57" s="39">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B57" s="5">
+        <f t="shared" ref="B57" si="18">IF(C57=C56,B56,B56+1)</f>
         <v>8</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C57" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="D55" s="5">
-        <f t="shared" ref="D55" si="15">IF(B55=B54,IF(E55=E54,D54,D54+1),1)</f>
+      <c r="D57" s="5">
+        <f t="shared" ref="D57" si="19">IF(B57=B56,IF(E57=E56,D56,D56+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E55" s="39" t="s">
+      <c r="E57" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F57" s="5">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="G55" s="39" t="s">
+      <c r="G57" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H57" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="I57" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="J55" s="5" t="s">
+      <c r="J57" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K55" s="6" t="s">
+      <c r="K57" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="L55" s="6"/>
-      <c r="M55" s="5" t="s">
+      <c r="L57" s="6"/>
+      <c r="M57" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="N55" s="32" t="s">
+      <c r="N57" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="O55" s="37" t="s">
+      <c r="O57" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P55" s="42"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="17">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B56" s="17">
-        <f>IF(C56=C53,B53,B53+1)</f>
+      <c r="P57" s="42"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58" s="17">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B58" s="17">
+        <f>IF(C58=C55,B55,B55+1)</f>
         <v>8</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C58" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="D56" s="17">
-        <f>IF(B56=B53,IF(E56=E53,D53,D53+1),1)</f>
+      <c r="D58" s="17">
+        <f>IF(B58=B55,IF(E58=E55,D55,D55+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E58" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F58" s="17">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G58" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H56" s="17" t="s">
+      <c r="H58" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="I56" s="17" t="s">
+      <c r="I58" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="J56" s="17" t="s">
+      <c r="J58" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="K56" s="17" t="s">
+      <c r="K58" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17" t="s">
+      <c r="L58" s="17"/>
+      <c r="M58" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="N56" s="17" t="s">
+      <c r="N58" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="O56" s="18"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A57" s="17">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B57" s="17">
+      <c r="O58" s="18"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59" s="17">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B59" s="17">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C59" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D59" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E59" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F57" s="17">
+      <c r="F59" s="17">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="G57" s="17" t="s">
+      <c r="G59" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="H57" s="17" t="s">
+      <c r="H59" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="I57" s="17" t="s">
+      <c r="I59" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="J57" s="17" t="s">
+      <c r="J59" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="K57" s="17" t="s">
+      <c r="K59" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17" t="s">
+      <c r="L59" s="17"/>
+      <c r="M59" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="N57" s="17" t="s">
+      <c r="N59" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="O57" s="18"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="5">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B58" s="5">
+      <c r="O59" s="18"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B60" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C60" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D60" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F60" s="5">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G60" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H60" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="I60" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="J58" s="5" t="s">
+      <c r="J60" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="K58" s="6" t="s">
+      <c r="K60" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="L58" s="6"/>
-      <c r="M58" s="5" t="s">
+      <c r="L60" s="6"/>
+      <c r="M60" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="N58" s="29" t="s">
+      <c r="N60" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="O58" s="37" t="s">
+      <c r="O60" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P58" s="42"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A59" s="39">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B59" s="5">
-        <f>IF(C59=C55,B55,B55+1)</f>
+      <c r="P60" s="42"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" s="39">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B61" s="5">
+        <f>IF(C61=C57,B57,B57+1)</f>
         <v>8</v>
       </c>
-      <c r="C59" s="39" t="s">
+      <c r="C61" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="D59" s="5">
-        <f>IF(B59=B55,IF(E59=E55,D55,D55+1),1)</f>
+      <c r="D61" s="5">
+        <f>IF(B61=B57,IF(E61=E57,D57,D57+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E59" s="39" t="s">
+      <c r="E61" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F59" s="5">
+      <c r="F61" s="5">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="G59" s="39" t="s">
+      <c r="G61" s="39" t="s">
         <v>282</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H61" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I61" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="J59" s="5" t="s">
+      <c r="J61" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K59" s="6" t="s">
+      <c r="K61" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="L59" s="6"/>
-      <c r="M59" s="5" t="s">
+      <c r="L61" s="6"/>
+      <c r="M61" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="N59" s="32" t="s">
+      <c r="N61" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="O59" s="37" t="s">
+      <c r="O61" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P59" s="42"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="5">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B60" s="5">
-        <f>IF(C60=C54,B54,B54+1)</f>
+      <c r="P61" s="42"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62" s="5">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B62" s="5">
+        <f>IF(C62=C56,B56,B56+1)</f>
         <v>8</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C62" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D60" s="5">
-        <f>IF(B60=B54,IF(E60=E54,D54,D54+1),1)</f>
+      <c r="D62" s="5">
+        <f>IF(B62=B56,IF(E62=E56,D56,D56+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E62" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="5">
+      <c r="F62" s="5">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G62" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="H60" s="5" t="s">
+      <c r="H62" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="I62" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="J62" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="K60" s="6" t="s">
+      <c r="K62" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="L60" s="6"/>
-      <c r="M60" s="5" t="s">
+      <c r="L62" s="6"/>
+      <c r="M62" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="N60" s="29" t="s">
+      <c r="N62" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="O60" s="37" t="s">
+      <c r="O62" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P60" s="42"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="17">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B61" s="17">
+      <c r="P62" s="42"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="17">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B63" s="17">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C63" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D63" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E61" s="18" t="s">
+      <c r="E63" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F63" s="17">
         <v>1</v>
       </c>
-      <c r="G61" s="18" t="s">
+      <c r="G63" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H61" s="17" t="s">
+      <c r="H63" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="I61" s="17" t="s">
+      <c r="I63" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J61" s="17" t="s">
+      <c r="J63" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="K61" s="17" t="s">
+      <c r="K63" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17" t="s">
+      <c r="L63" s="17"/>
+      <c r="M63" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="N61" s="17" t="s">
+      <c r="N63" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="O61" s="18"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="5">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B62" s="5">
+      <c r="O63" s="18"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" s="5">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B64" s="5">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C64" s="15" t="s">
         <v>19</v>
-      </c>
-      <c r="D62" s="5">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E62" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="5">
-        <v>1</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="K62" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="L62" s="6"/>
-      <c r="M62" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N62" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="O62" s="37" t="s">
-        <v>278</v>
-      </c>
-      <c r="P62" s="42"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="5">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B63" s="5">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D63" s="5">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F63" s="5">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="L63" s="6"/>
-      <c r="M63" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="N63" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="O63" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P63" s="42"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="5">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B64" s="5">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>20</v>
       </c>
       <c r="D64" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>63</v>
+      <c r="E64" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="F64" s="5">
         <v>1</v>
@@ -6649,75 +6697,73 @@
         <v>5</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>263</v>
+        <v>44</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="L64" s="6" t="s">
-        <v>310</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="L64" s="6"/>
       <c r="M64" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="N64" s="34" t="s">
-        <v>257</v>
+        <v>185</v>
+      </c>
+      <c r="N64" s="23" t="s">
+        <v>230</v>
       </c>
       <c r="O64" s="37" t="s">
-        <v>12</v>
+        <v>278</v>
       </c>
       <c r="P64" s="42"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="39">
+      <c r="A65" s="5">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B65" s="39">
+      <c r="B65" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="C65" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65" s="39">
+        <v>10</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E65" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="F65" s="39">
+      <c r="E65" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G65" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H65" s="39" t="s">
-        <v>343</v>
-      </c>
-      <c r="I65" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="J65" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="K65" s="39" t="s">
-        <v>347</v>
-      </c>
-      <c r="L65" s="39"/>
-      <c r="M65" s="39" t="s">
-        <v>348</v>
-      </c>
-      <c r="N65" s="32" t="s">
-        <v>288</v>
+      <c r="G65" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="L65" s="6"/>
+      <c r="M65" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="N65" s="19" t="s">
+        <v>229</v>
       </c>
       <c r="O65" s="37" t="s">
         <v>12</v>
@@ -6744,535 +6790,533 @@
         <v>63</v>
       </c>
       <c r="F66" s="5">
+        <v>1</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="L66" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="N66" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="O66" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P66" s="42"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A67" s="39">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B67" s="39">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C67" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F67" s="39">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="G67" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="I67" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="J67" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="K67" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="L67" s="39"/>
+      <c r="M67" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="N67" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="O67" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P67" s="42"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A68" s="5">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B68" s="5">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F68" s="5">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G68" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H68" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I68" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="J66" s="5" t="s">
+      <c r="J68" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="K66" s="6" t="s">
+      <c r="K68" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L66" s="6" t="s">
+      <c r="L68" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="M66" s="5" t="s">
+      <c r="M68" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="N66" s="45" t="s">
+      <c r="N68" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="O66" s="37" t="s">
+      <c r="O68" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P66" s="42"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A67" s="5">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B67" s="5">
+      <c r="P68" s="42"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A69" s="5">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B69" s="5">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C69" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D69" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F67" s="5">
+      <c r="F69" s="5">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="G67" s="5" t="s">
+      <c r="G69" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H69" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I69" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="J67" s="5" t="s">
+      <c r="J69" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="K67" s="6" t="s">
+      <c r="K69" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="L67" s="6" t="s">
+      <c r="L69" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="M67" s="5" t="s">
+      <c r="M69" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="N67" s="34" t="s">
+      <c r="N69" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="O67" s="37" t="s">
+      <c r="O69" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P67" s="42"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A68" s="5">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B68" s="5">
-        <f t="shared" ref="B68" si="16">IF(C68=C67,B67,B67+1)</f>
+      <c r="P69" s="42"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A70" s="5">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B70" s="5">
+        <f t="shared" ref="B70" si="20">IF(C70=C69,B69,B69+1)</f>
         <v>11</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C70" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="5">
-        <f t="shared" ref="D68" si="17">IF(B68=B67,IF(E68=E67,D67,D67+1),1)</f>
+      <c r="D70" s="5">
+        <f t="shared" ref="D70" si="21">IF(B70=B69,IF(E70=E69,D69,D69+1),1)</f>
         <v>1</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F68" s="5">
+      <c r="F70" s="5">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="G68" s="5" t="s">
+      <c r="G70" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H70" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I70" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="J68" s="5" t="s">
+      <c r="J70" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="K68" s="6" t="s">
+      <c r="K70" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="L68" s="9" t="s">
+      <c r="L70" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="M68" s="5" t="s">
+      <c r="M70" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="N68" s="34" t="s">
+      <c r="N70" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="O68" s="37" t="s">
+      <c r="O70" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P68" s="42"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A69" s="5">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B69" s="5">
-        <f t="shared" ref="B69" si="18">IF(C69=C68,B68,B68+1)</f>
+      <c r="P70" s="42"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A71" s="5">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B71" s="5">
+        <f t="shared" ref="B71" si="22">IF(C71=C70,B70,B70+1)</f>
         <v>11</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C71" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D69" s="5">
-        <f t="shared" ref="D69" si="19">IF(B69=B68,IF(E69=E68,D68,D68+1),1)</f>
+      <c r="D71" s="5">
+        <f t="shared" ref="D71" si="23">IF(B71=B70,IF(E71=E70,D70,D70+1),1)</f>
         <v>1</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F69" s="5">
+      <c r="F71" s="5">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G71" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="H71" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I71" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="J71" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="K69" s="6" t="s">
+      <c r="K71" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L71" t="s">
         <v>325</v>
       </c>
-      <c r="M69" s="5" t="s">
+      <c r="M71" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="N69" s="34" t="s">
+      <c r="N71" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="O69" s="37" t="s">
+      <c r="O71" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P69" s="42"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A70" s="17">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B70" s="17">
-        <f>IF(C70=C67,B67,B67+1)</f>
+      <c r="P71" s="42"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" s="17">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B72" s="17">
+        <f>IF(C72=C69,B69,B69+1)</f>
         <v>11</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C72" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="17">
-        <f>IF(B70=B67,IF(E70=E67,D67,D67+1),1)</f>
+      <c r="D72" s="17">
+        <f>IF(B72=B69,IF(E72=E69,D69,D69+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E72" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F70" s="17">
+      <c r="F72" s="17">
         <v>1</v>
       </c>
-      <c r="G70" s="17" t="s">
+      <c r="G72" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H70" s="17" t="s">
+      <c r="H72" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="I70" s="17" t="s">
+      <c r="I72" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="J70" s="17" t="s">
+      <c r="J72" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="K70" s="17" t="s">
+      <c r="K72" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="L70" s="17"/>
-      <c r="M70" s="17" t="s">
+      <c r="L72" s="17"/>
+      <c r="M72" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="N70" s="17" t="s">
+      <c r="N72" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="O70" s="18"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A71" s="5">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="B71" s="5">
+      <c r="O72" s="18"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A73" s="5">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B73" s="5">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C73" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="5">
+      <c r="D73" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E73" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F71" s="5">
+      <c r="F73" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G71" s="6" t="s">
+      <c r="G73" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H73" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I73" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="J71" s="5" t="s">
+      <c r="J73" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="K71" s="6" t="s">
+      <c r="K73" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L71" s="6"/>
-      <c r="M71" s="5" t="s">
+      <c r="L73" s="6"/>
+      <c r="M73" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="N71" s="29" t="s">
+      <c r="N73" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="O71" s="37" t="s">
+      <c r="O73" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P71" s="42"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A72" s="39">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="B72" s="39">
+      <c r="P73" s="42"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A74" s="39">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B74" s="39">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="C74" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="39">
+      <c r="D74" s="39">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E72" s="39" t="s">
+      <c r="E74" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F72" s="39">
+      <c r="F74" s="39">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="G72" s="40" t="s">
+      <c r="G74" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="H72" s="39" t="s">
+      <c r="H74" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="I72" s="39" t="s">
+      <c r="I74" s="39" t="s">
         <v>332</v>
       </c>
-      <c r="J72" s="39" t="s">
+      <c r="J74" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="K72" s="39" t="s">
+      <c r="K74" s="39" t="s">
         <v>345</v>
       </c>
-      <c r="L72" s="39"/>
-      <c r="M72" s="39" t="s">
+      <c r="L74" s="39"/>
+      <c r="M74" s="39" t="s">
         <v>346</v>
       </c>
-      <c r="N72" s="32" t="s">
+      <c r="N74" s="32" t="s">
         <v>288</v>
       </c>
-      <c r="O72" s="37" t="s">
+      <c r="O74" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P72" s="42"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A73" s="17">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="B73" s="17">
-        <f t="shared" ref="B73" si="20">IF(C73=C72,B72,B72+1)</f>
+      <c r="P74" s="42"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75" s="17">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B75" s="17">
+        <f t="shared" ref="B75" si="24">IF(C75=C74,B74,B74+1)</f>
         <v>11</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="C75" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="17">
-        <f t="shared" ref="D73" si="21">IF(B73=B72,IF(E73=E72,D72,D72+1),1)</f>
+      <c r="D75" s="17">
+        <f t="shared" ref="D75" si="25">IF(B75=B74,IF(E75=E74,D74,D74+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E75" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F73" s="17">
+      <c r="F75" s="17">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="G73" s="17" t="s">
+      <c r="G75" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="H73" s="17" t="s">
+      <c r="H75" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="I73" s="17" t="s">
+      <c r="I75" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="J73" s="17" t="s">
+      <c r="J75" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="K73" s="17" t="s">
+      <c r="K75" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17" t="s">
+      <c r="L75" s="17"/>
+      <c r="M75" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="N73" s="17" t="s">
+      <c r="N75" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="O73" s="18"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A74" s="5">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="B74" s="5">
-        <f>IF(C74=C72,B72,B72+1)</f>
-        <v>11</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D74" s="5">
-        <f>IF(B74=B72,IF(E74=E72,D72,D72+1),1)</f>
-        <v>3</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F74" s="5">
-        <v>1</v>
-      </c>
-      <c r="G74" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="K74" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="L74" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="M74" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="N74" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="O74" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P74" s="42"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A75" s="5">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="B75" s="5">
-        <f>IF(C75=C73,B73,B73+1)</f>
-        <v>11</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D75" s="5">
-        <f>IF(B75=B73,IF(E75=E73,D73,D73+1),1)</f>
-        <v>3</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F75" s="5">
-        <v>1</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K75" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="L75" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="M75" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="N75" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="O75" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P75" s="42"/>
+      <c r="O75" s="18"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
-        <f t="shared" ref="A76:A82" si="22">ROW()-4</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="B76" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C76=C74,B74,B74+1)</f>
         <v>11</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D76" s="5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>IF(B76=B74,IF(E76=E74,D74,D74+1),1)</f>
+        <v>3</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F76" s="5">
-        <f t="shared" ref="F76:F79" si="23">F75+1</f>
-        <v>2</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>47</v>
+        <v>1</v>
+      </c>
+      <c r="G76" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>47</v>
+        <v>353</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>152</v>
+        <v>305</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="L76" s="39" t="s">
-        <v>313</v>
+        <v>161</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="M76" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="N76" s="23" t="s">
-        <v>230</v>
+        <v>354</v>
+      </c>
+      <c r="N76" s="25" t="s">
+        <v>247</v>
       </c>
       <c r="O76" s="37" t="s">
         <v>12</v>
@@ -7281,50 +7325,49 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="B77" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C77=C75,B75,B75+1)</f>
         <v>11</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D77" s="5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>IF(B77=B75,IF(E77=E75,D75,D75+1),1)</f>
+        <v>3</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F77" s="5">
-        <f t="shared" si="23"/>
-        <v>3</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="G77" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>48</v>
+        <v>178</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>153</v>
+        <v>355</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="L77" s="39" t="s">
-        <v>313</v>
+        <v>161</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="M77" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="N77" s="23" t="s">
-        <v>230</v>
+        <v>188</v>
+      </c>
+      <c r="N77" s="25" t="s">
+        <v>247</v>
       </c>
       <c r="O77" s="37" t="s">
         <v>12</v>
@@ -7333,7 +7376,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="A78:A84" si="26">ROW()-4</f>
         <v>74</v>
       </c>
       <c r="B78" s="5">
@@ -7351,29 +7394,29 @@
         <v>26</v>
       </c>
       <c r="F78" s="5">
-        <f t="shared" si="23"/>
-        <v>4</v>
+        <f t="shared" ref="F78:F81" si="27">F77+1</f>
+        <v>2</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>342</v>
+        <v>47</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="L78" s="39" t="s">
         <v>313</v>
       </c>
       <c r="M78" s="5" t="s">
-        <v>183</v>
+        <v>224</v>
       </c>
       <c r="N78" s="23" t="s">
         <v>230</v>
@@ -7385,7 +7428,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>75</v>
       </c>
       <c r="B79" s="5">
@@ -7403,29 +7446,29 @@
         <v>26</v>
       </c>
       <c r="F79" s="5">
-        <f t="shared" si="23"/>
-        <v>5</v>
+        <f t="shared" si="27"/>
+        <v>3</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>294</v>
+        <v>153</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L79" s="39" t="s">
         <v>313</v>
       </c>
       <c r="M79" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N79" s="23" t="s">
         <v>230</v>
@@ -7437,7 +7480,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>76</v>
       </c>
       <c r="B80" s="5">
@@ -7449,37 +7492,38 @@
       </c>
       <c r="D80" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F80" s="5">
-        <v>1</v>
-      </c>
-      <c r="G80" s="16" t="s">
-        <v>5</v>
+        <f t="shared" si="27"/>
+        <v>4</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="L80" s="6" t="s">
-        <v>314</v>
+        <v>179</v>
+      </c>
+      <c r="L80" s="39" t="s">
+        <v>313</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="N80" s="24" t="s">
-        <v>231</v>
+        <v>183</v>
+      </c>
+      <c r="N80" s="23" t="s">
+        <v>230</v>
       </c>
       <c r="O80" s="37" t="s">
         <v>12</v>
@@ -7488,7 +7532,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>77</v>
       </c>
       <c r="B81" s="5">
@@ -7500,37 +7544,38 @@
       </c>
       <c r="D81" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F81" s="5">
-        <v>1</v>
-      </c>
-      <c r="G81" s="16" t="s">
+        <f t="shared" si="27"/>
         <v>5</v>
       </c>
+      <c r="G81" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="H81" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>155</v>
+        <v>294</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="L81" s="6" t="s">
-        <v>315</v>
+        <v>162</v>
+      </c>
+      <c r="L81" s="39" t="s">
+        <v>313</v>
       </c>
       <c r="M81" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="N81" s="41" t="s">
-        <v>232</v>
+        <v>184</v>
+      </c>
+      <c r="N81" s="23" t="s">
+        <v>230</v>
       </c>
       <c r="O81" s="37" t="s">
         <v>12</v>
@@ -7539,7 +7584,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>78</v>
       </c>
       <c r="B82" s="5">
@@ -7551,10 +7596,10 @@
       </c>
       <c r="D82" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F82" s="5">
         <v>1</v>
@@ -7563,23 +7608,25 @@
         <v>5</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="L82" s="6"/>
+        <v>356</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="M82" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="N82" s="34" t="s">
-        <v>257</v>
+        <v>186</v>
+      </c>
+      <c r="N82" s="24" t="s">
+        <v>231</v>
       </c>
       <c r="O82" s="37" t="s">
         <v>12</v>
@@ -7587,18 +7634,104 @@
       <c r="P82" s="42"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
+      <c r="A83" s="5">
+        <f t="shared" si="26"/>
+        <v>79</v>
+      </c>
+      <c r="B83" s="5">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" s="5">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" s="5">
+        <v>1</v>
+      </c>
+      <c r="G83" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K83" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L83" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="M83" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="N83" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="O83" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P83" s="42"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
+      <c r="A84" s="5">
+        <f t="shared" si="26"/>
+        <v>80</v>
+      </c>
+      <c r="B84" s="5">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" s="5">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" s="5">
+        <v>1</v>
+      </c>
+      <c r="G84" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K84" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="L84" s="6"/>
+      <c r="M84" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="N84" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="O84" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P84" s="42"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B85" s="4"/>
@@ -7838,8 +7971,22 @@
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
     </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:N82"/>
+  <autoFilter ref="A4:N84"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added post notice mail feature.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/APIList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/APIList.xlsx
@@ -1677,10 +1677,6 @@
     <t>searchPathsAction($slug)</t>
   </si>
   <si>
-    <t>AH0206</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>AM0202</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2363,6 +2359,10 @@
   </si>
   <si>
     <t>getOkrDescendantsAction($slug)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AH0209</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3168,12 +3168,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="48.5" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3835,20 +3835,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="18" style="3" customWidth="1"/>
-    <col min="4" max="4" width="4.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="4.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="59.1640625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="12.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="59.140625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="39" style="3" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" style="3" customWidth="1"/>
     <col min="13" max="13" width="39" style="3" customWidth="1"/>
-    <col min="14" max="14" width="46.1640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="38"/>
+    <col min="14" max="14" width="46.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="38" x14ac:dyDescent="0.55000000000000004">
@@ -4272,7 +4272,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>121</v>
@@ -4443,7 +4443,7 @@
       </c>
       <c r="P14" s="42"/>
     </row>
-    <row r="15" spans="1:17" ht="40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="P15" s="42"/>
     </row>
-    <row r="16" spans="1:17" ht="40" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="P16" s="42"/>
     </row>
-    <row r="17" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4592,7 +4592,7 @@
       </c>
       <c r="P17" s="42"/>
     </row>
-    <row r="18" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4639,7 +4639,7 @@
       </c>
       <c r="O18" s="37"/>
     </row>
-    <row r="19" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="O19" s="37"/>
     </row>
-    <row r="20" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="P20" s="42"/>
     </row>
-    <row r="21" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="P21" s="42"/>
     </row>
-    <row r="22" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4810,7 +4810,7 @@
         <v>8</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>73</v>
@@ -4836,7 +4836,7 @@
       </c>
       <c r="P22" s="42"/>
     </row>
-    <row r="23" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -4860,7 +4860,7 @@
         <v>9</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>74</v>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="P23" s="42"/>
     </row>
-    <row r="24" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -4946,14 +4946,14 @@
         <v>5</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D25" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F25" s="17">
         <f t="shared" si="5"/>
@@ -4972,11 +4972,11 @@
         <v>113</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N25" s="17" t="s">
         <v>282</v>
@@ -5013,20 +5013,20 @@
         <v>38</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N26" s="32" t="s">
         <v>282</v>
@@ -5036,7 +5036,7 @@
       </c>
       <c r="P26" s="42"/>
     </row>
-    <row r="27" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5063,7 +5063,7 @@
         <v>38</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>133</v>
@@ -5072,11 +5072,11 @@
         <v>60</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N27" s="32" t="s">
         <v>282</v>
@@ -5086,7 +5086,7 @@
       </c>
       <c r="P27" s="42"/>
     </row>
-    <row r="28" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="P28" s="42"/>
     </row>
-    <row r="29" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5166,7 +5166,7 @@
         <v>285</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>60</v>
@@ -5186,7 +5186,7 @@
       </c>
       <c r="P29" s="42"/>
     </row>
-    <row r="30" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5216,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>101</v>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="L30" s="6"/>
       <c r="M30" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N30" s="33" t="s">
         <v>250</v>
@@ -5246,20 +5246,20 @@
         <v>6</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D31" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F31" s="17">
         <v>1</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H31" s="17" t="s">
         <v>30</v>
@@ -5268,14 +5268,14 @@
         <v>134</v>
       </c>
       <c r="J31" s="17" t="s">
+        <v>433</v>
+      </c>
+      <c r="K31" s="17" t="s">
         <v>434</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>435</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N31" s="17" t="s">
         <v>243</v>
@@ -5311,20 +5311,20 @@
         <v>5</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N32" s="26" t="s">
         <v>243</v>
@@ -5340,24 +5340,24 @@
         <v>29</v>
       </c>
       <c r="B33" s="17">
-        <f>IF(C33=C31,B31,B31+1)</f>
+        <f t="shared" ref="B33:B39" si="12">IF(C33=C31,B31,B31+1)</f>
         <v>6</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D33" s="17">
-        <f>IF(B33=B31,IF(E33=E31,D31,D31+1),1)</f>
+        <f t="shared" ref="D33:D39" si="13">IF(B33=B31,IF(E33=E31,D31,D31+1),1)</f>
         <v>2</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F33" s="17">
         <v>1</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>32</v>
@@ -5366,14 +5366,14 @@
         <v>135</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K33" s="17" t="s">
         <v>102</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N33" s="17" t="s">
         <v>243</v>
@@ -5389,14 +5389,14 @@
         <v>30</v>
       </c>
       <c r="B34" s="5">
-        <f>IF(C34=C32,B32,B32+1)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D34" s="5">
-        <f>IF(B34=B32,IF(E34=E32,D32,D32+1),1)</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -5409,20 +5409,20 @@
         <v>5</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N34" s="26" t="s">
         <v>243</v>
@@ -5438,14 +5438,14 @@
         <v>31</v>
       </c>
       <c r="B35" s="17">
-        <f>IF(C35=C33,B33,B33+1)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D35" s="17">
-        <f>IF(B35=B33,IF(E35=E33,D33,D33+1),1)</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="E35" s="17" t="s">
@@ -5455,23 +5455,23 @@
         <v>1</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>33</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K35" s="17" t="s">
         <v>103</v>
       </c>
       <c r="L35" s="17"/>
       <c r="M35" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N35" s="17" t="s">
         <v>243</v>
@@ -5487,14 +5487,14 @@
         <v>32</v>
       </c>
       <c r="B36" s="5">
-        <f>IF(C36=C34,B34,B34+1)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="5">
-        <f>IF(B36=B34,IF(E36=E34,D34,D34+1),1)</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="E36" s="5" t="s">
@@ -5507,20 +5507,20 @@
         <v>5</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N36" s="26" t="s">
         <v>243</v>
@@ -5530,30 +5530,30 @@
       </c>
       <c r="P36" s="42"/>
     </row>
-    <row r="37" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B37" s="17">
-        <f>IF(C37=C35,B35,B35+1)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D37" s="17">
-        <f>IF(B37=B35,IF(E37=E35,D35,D35+1),1)</f>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F37" s="17">
         <v>1</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>273</v>
@@ -5562,14 +5562,14 @@
         <v>136</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K37" s="17" t="s">
         <v>104</v>
       </c>
       <c r="L37" s="17"/>
       <c r="M37" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="N37" s="17" t="s">
         <v>243</v>
@@ -5579,24 +5579,24 @@
       </c>
       <c r="P37" s="42"/>
     </row>
-    <row r="38" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B38" s="5">
-        <f>IF(C38=C36,B36,B36+1)</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D38" s="5">
-        <f>IF(B38=B36,IF(E38=E36,D36,D36+1),1)</f>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F38" s="5">
         <v>1</v>
@@ -5605,20 +5605,20 @@
         <v>5</v>
       </c>
       <c r="H38" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="I38" s="5" t="s">
         <v>446</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>447</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L38" s="6"/>
       <c r="M38" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N38" s="26" t="s">
         <v>243</v>
@@ -5634,14 +5634,14 @@
         <v>35</v>
       </c>
       <c r="B39" s="5">
-        <f>IF(C39=C37,B37,B37+1)</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="5">
-        <f>IF(B39=B37,IF(E39=E37,D37,D37+1),1)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -5654,7 +5654,7 @@
         <v>5</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>137</v>
@@ -5704,7 +5704,7 @@
         <v>5</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>138</v>
@@ -5744,7 +5744,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F41" s="5">
         <v>1</v>
@@ -5753,20 +5753,20 @@
         <v>5</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J41" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L41" s="6"/>
       <c r="M41" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N41" s="27" t="s">
         <v>229</v>
@@ -5789,11 +5789,11 @@
         <v>17</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" ref="D42:D45" si="12">IF(B42=B40,IF(E42=E40,D40,D40+1),1)</f>
+        <f t="shared" ref="D42:D45" si="14">IF(B42=B40,IF(E42=E40,D40,D40+1),1)</f>
         <v>2</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F42" s="5">
         <f>F41+1</f>
@@ -5803,20 +5803,20 @@
         <v>5</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J42" s="5" t="s">
         <v>94</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N42" s="27" t="s">
         <v>229</v>
@@ -5839,11 +5839,11 @@
         <v>17</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F43" s="5">
         <v>1</v>
@@ -5852,10 +5852,10 @@
         <v>5</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>94</v>
@@ -5888,11 +5888,11 @@
         <v>17</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F44" s="5">
         <f>F43+1</f>
@@ -5905,7 +5905,7 @@
         <v>82</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>94</v>
@@ -5931,18 +5931,18 @@
         <v>41</v>
       </c>
       <c r="B45" s="5">
-        <f t="shared" ref="B45" si="13">IF(C45=C44,B44,B44+1)</f>
+        <f t="shared" ref="B45" si="15">IF(C45=C44,B44,B44+1)</f>
         <v>7</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F45" s="5">
         <f>F44+1</f>
@@ -5955,7 +5955,7 @@
         <v>291</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>111</v>
@@ -5981,18 +5981,18 @@
         <v>42</v>
       </c>
       <c r="B46" s="5">
-        <f t="shared" ref="B46" si="14">IF(C46=C45,B45,B45+1)</f>
+        <f t="shared" ref="B46" si="16">IF(C46=C45,B45,B45+1)</f>
         <v>7</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" ref="D46" si="15">IF(B46=B44,IF(E46=E44,D44,D44+1),1)</f>
+        <f t="shared" ref="D46" si="17">IF(B46=B44,IF(E46=E44,D44,D44+1),1)</f>
         <v>3</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F46" s="5">
         <f>F45+1</f>
@@ -6002,20 +6002,20 @@
         <v>5</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>111</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L46" s="6"/>
       <c r="M46" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N46" s="27" t="s">
         <v>229</v>
@@ -6031,18 +6031,18 @@
         <v>43</v>
       </c>
       <c r="B47" s="5">
-        <f t="shared" ref="B47" si="16">IF(C47=C46,B46,B46+1)</f>
+        <f t="shared" ref="B47" si="18">IF(C47=C46,B46,B46+1)</f>
         <v>7</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" ref="D47" si="17">IF(B47=B45,IF(E47=E45,D45,D45+1),1)</f>
+        <f t="shared" ref="D47" si="19">IF(B47=B45,IF(E47=E45,D45,D45+1),1)</f>
         <v>3</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F47" s="5">
         <f>F46+1</f>
@@ -6052,20 +6052,20 @@
         <v>5</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J47" s="5" t="s">
         <v>101</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L47" s="6"/>
       <c r="M47" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N47" s="27" t="s">
         <v>229</v>
@@ -6214,7 +6214,7 @@
       </c>
       <c r="L50" s="17"/>
       <c r="M50" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="N50" s="17" t="s">
         <v>282</v>
@@ -6251,7 +6251,7 @@
         <v>83</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I51" s="5" t="s">
         <v>141</v>
@@ -6260,11 +6260,11 @@
         <v>60</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N51" s="32" t="s">
         <v>282</v>
@@ -6348,13 +6348,13 @@
         <v>6</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>87</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>111</v>
@@ -6529,14 +6529,14 @@
         <v>53</v>
       </c>
       <c r="B57" s="5">
-        <f t="shared" ref="B57" si="18">IF(C57=C56,B56,B56+1)</f>
+        <f t="shared" ref="B57" si="20">IF(C57=C56,B56,B56+1)</f>
         <v>8</v>
       </c>
       <c r="C57" s="39" t="s">
         <v>81</v>
       </c>
       <c r="D57" s="5">
-        <f t="shared" ref="D57" si="19">IF(B57=B56,IF(E57=E56,D56,D56+1),1)</f>
+        <f t="shared" ref="D57" si="21">IF(B57=B56,IF(E57=E56,D56,D56+1),1)</f>
         <v>2</v>
       </c>
       <c r="E57" s="39" t="s">
@@ -6550,20 +6550,20 @@
         <v>41</v>
       </c>
       <c r="H57" s="39" t="s">
+        <v>380</v>
+      </c>
+      <c r="I57" s="39" t="s">
         <v>381</v>
-      </c>
-      <c r="I57" s="39" t="s">
-        <v>382</v>
       </c>
       <c r="J57" s="39" t="s">
         <v>253</v>
       </c>
       <c r="K57" s="39" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L57" s="39"/>
       <c r="M57" s="39" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N57" s="32" t="s">
         <v>282</v>
@@ -6647,7 +6647,7 @@
         <v>6</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>245</v>
@@ -6729,14 +6729,14 @@
         <v>57</v>
       </c>
       <c r="B61" s="5">
-        <f t="shared" ref="B61" si="20">IF(C61=C60,B60,B60+1)</f>
+        <f t="shared" ref="B61" si="22">IF(C61=C60,B60,B60+1)</f>
         <v>8</v>
       </c>
       <c r="C61" s="39" t="s">
         <v>277</v>
       </c>
       <c r="D61" s="5">
-        <f t="shared" ref="D61" si="21">IF(B61=B60,IF(E61=E60,D60,D60+1),1)</f>
+        <f t="shared" ref="D61" si="23">IF(B61=B60,IF(E61=E60,D60,D60+1),1)</f>
         <v>2</v>
       </c>
       <c r="E61" s="39" t="s">
@@ -6750,20 +6750,20 @@
         <v>42</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L61" s="6"/>
       <c r="M61" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="N61" s="32" t="s">
         <v>282</v>
@@ -6844,13 +6844,13 @@
         <v>10</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H63" s="17" t="s">
         <v>87</v>
       </c>
       <c r="I63" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J63" s="17" t="s">
         <v>111</v>
@@ -6891,13 +6891,13 @@
         <v>11</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>111</v>
@@ -6944,20 +6944,20 @@
         <v>276</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>60</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L65" s="6"/>
       <c r="M65" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N65" s="32" t="s">
         <v>282</v>
@@ -6997,7 +6997,7 @@
         <v>276</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>278</v>
@@ -7148,11 +7148,11 @@
         <v>94</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L69" s="6"/>
       <c r="M69" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N69" s="19" t="s">
         <v>223</v>
@@ -7240,7 +7240,7 @@
         <v>5</v>
       </c>
       <c r="H71" s="39" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I71" s="39" t="s">
         <v>233</v>
@@ -7249,11 +7249,11 @@
         <v>113</v>
       </c>
       <c r="K71" s="39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L71" s="39"/>
       <c r="M71" s="39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="N71" s="32" t="s">
         <v>282</v>
@@ -7287,7 +7287,7 @@
         <v>3</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>232</v>
@@ -7339,7 +7339,7 @@
         <v>4</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>302</v>
@@ -7373,14 +7373,14 @@
         <v>70</v>
       </c>
       <c r="B74" s="5">
-        <f t="shared" ref="B74" si="22">IF(C74=C73,B73,B73+1)</f>
+        <f t="shared" ref="B74" si="24">IF(C74=C73,B73,B73+1)</f>
         <v>11</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="5">
-        <f t="shared" ref="D74" si="23">IF(B74=B73,IF(E74=E73,D73,D73+1),1)</f>
+        <f t="shared" ref="D74" si="25">IF(B74=B73,IF(E74=E73,D73,D73+1),1)</f>
         <v>1</v>
       </c>
       <c r="E74" s="5" t="s">
@@ -7425,14 +7425,14 @@
         <v>71</v>
       </c>
       <c r="B75" s="5">
-        <f t="shared" ref="B75" si="24">IF(C75=C74,B74,B74+1)</f>
+        <f t="shared" ref="B75" si="26">IF(C75=C74,B74,B74+1)</f>
         <v>11</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" ref="D75" si="25">IF(B75=B74,IF(E75=E74,D74,D74+1),1)</f>
+        <f t="shared" ref="D75" si="27">IF(B75=B74,IF(E75=E74,D74,D74+1),1)</f>
         <v>1</v>
       </c>
       <c r="E75" s="5" t="s">
@@ -7449,7 +7449,7 @@
         <v>311</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J75" s="5" t="s">
         <v>101</v>
@@ -7594,20 +7594,20 @@
         <v>5</v>
       </c>
       <c r="H78" s="39" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I78" s="39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J78" s="39" t="s">
         <v>113</v>
       </c>
       <c r="K78" s="39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L78" s="39"/>
       <c r="M78" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N78" s="32" t="s">
         <v>282</v>
@@ -7623,14 +7623,14 @@
         <v>75</v>
       </c>
       <c r="B79" s="17">
-        <f t="shared" ref="B79" si="26">IF(C79=C78,B78,B78+1)</f>
+        <f t="shared" ref="B79" si="28">IF(C79=C78,B78,B78+1)</f>
         <v>11</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D79" s="17">
-        <f t="shared" ref="D79" si="27">IF(B79=B78,IF(E79=E78,D78,D78+1),1)</f>
+        <f t="shared" ref="D79" si="29">IF(B79=B78,IF(E79=E78,D78,D78+1),1)</f>
         <v>2</v>
       </c>
       <c r="E79" s="17" t="s">
@@ -7641,13 +7641,13 @@
         <v>4</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H79" s="17" t="s">
         <v>43</v>
       </c>
       <c r="I79" s="17" t="s">
-        <v>325</v>
+        <v>449</v>
       </c>
       <c r="J79" s="17" t="s">
         <v>111</v>
@@ -7690,7 +7690,7 @@
         <v>5</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>299</v>
@@ -7705,7 +7705,7 @@
         <v>306</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N80" s="25" t="s">
         <v>241</v>
@@ -7744,7 +7744,7 @@
         <v>176</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J81" s="5" t="s">
         <v>101</v>
@@ -7766,9 +7766,9 @@
       </c>
       <c r="P81" s="42"/>
     </row>
-    <row r="82" spans="1:16" ht="40" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
-        <f t="shared" ref="A82:A91" si="28">ROW()-4</f>
+        <f t="shared" ref="A82:A91" si="30">ROW()-4</f>
         <v>78</v>
       </c>
       <c r="B82" s="5">
@@ -7786,7 +7786,7 @@
         <v>26</v>
       </c>
       <c r="F82" s="5">
-        <f t="shared" ref="F82:F85" si="29">F81+1</f>
+        <f t="shared" ref="F82:F85" si="31">F81+1</f>
         <v>2</v>
       </c>
       <c r="G82" s="5" t="s">
@@ -7820,7 +7820,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>79</v>
       </c>
       <c r="B83" s="5">
@@ -7838,7 +7838,7 @@
         <v>26</v>
       </c>
       <c r="F83" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>3</v>
       </c>
       <c r="G83" s="5" t="s">
@@ -7872,7 +7872,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>80</v>
       </c>
       <c r="B84" s="5">
@@ -7890,11 +7890,11 @@
         <v>26</v>
       </c>
       <c r="F84" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>4</v>
@@ -7924,7 +7924,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>81</v>
       </c>
       <c r="B85" s="5">
@@ -7942,7 +7942,7 @@
         <v>26</v>
       </c>
       <c r="F85" s="5">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="G85" s="5" t="s">
@@ -7976,7 +7976,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>82</v>
       </c>
       <c r="B86" s="5">
@@ -8009,7 +8009,7 @@
         <v>113</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L86" s="6" t="s">
         <v>308</v>
@@ -8027,7 +8027,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>83</v>
       </c>
       <c r="B87" s="5">
@@ -8078,7 +8078,7 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>84</v>
       </c>
       <c r="B88" s="5">
@@ -8127,22 +8127,22 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>85</v>
       </c>
       <c r="B89" s="5">
-        <f t="shared" ref="B89" si="30">IF(C89=C88,B88,B88+1)</f>
+        <f t="shared" ref="B89" si="32">IF(C89=C88,B88,B88+1)</f>
         <v>12</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D89" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F89" s="5">
         <v>1</v>
@@ -8151,23 +8151,23 @@
         <v>5</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J89" s="5" t="s">
         <v>94</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L89" s="6"/>
       <c r="M89" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N89" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O89" s="37" t="s">
         <v>12</v>
@@ -8176,22 +8176,22 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>86</v>
       </c>
       <c r="B90" s="5">
-        <f t="shared" ref="B90" si="31">IF(C90=C89,B89,B89+1)</f>
+        <f t="shared" ref="B90" si="33">IF(C90=C89,B89,B89+1)</f>
         <v>12</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D90" s="5">
-        <f t="shared" ref="D90" si="32">IF(B90=B89,IF(E90=E89,D89,D89+1),1)</f>
+        <f t="shared" ref="D90" si="34">IF(B90=B89,IF(E90=E89,D89,D89+1),1)</f>
         <v>1</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F90" s="5">
         <v>1</v>
@@ -8200,23 +8200,23 @@
         <v>5</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>94</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="L90" s="6"/>
       <c r="M90" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N90" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O90" s="37" t="s">
         <v>12</v>
@@ -8225,22 +8225,22 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>87</v>
       </c>
       <c r="B91" s="5">
-        <f t="shared" ref="B91" si="33">IF(C91=C90,B90,B90+1)</f>
+        <f t="shared" ref="B91" si="35">IF(C91=C90,B90,B90+1)</f>
         <v>12</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D91" s="5">
-        <f t="shared" ref="D91" si="34">IF(B91=B90,IF(E91=E90,D90,D90+1),1)</f>
+        <f t="shared" ref="D91" si="36">IF(B91=B90,IF(E91=E90,D90,D90+1),1)</f>
         <v>1</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F91" s="5">
         <v>1</v>
@@ -8249,23 +8249,23 @@
         <v>5</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J91" s="5" t="s">
         <v>94</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L91" s="6"/>
       <c r="M91" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N91" s="46" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O91" s="37" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
AE0404 CloneOKR - A new feature.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/APIList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/APIList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="27580" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1120" yWindow="460" windowWidth="27680" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="更新履歴" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="465">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -241,16 +241,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>OKRの複製・移動</t>
-    <rPh sb="4" eb="6">
-      <t>フクセ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>イド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>KRの加重平均割合設定</t>
     <rPh sb="3" eb="7">
       <t>カジュウヘイキn</t>
@@ -381,9 +371,6 @@
     <t>/api/okrs/{slug}.json</t>
   </si>
   <si>
-    <t>/api/okrs/{slug}/clone.json</t>
-  </si>
-  <si>
     <t>/api/okrs/{slug}/move.json</t>
   </si>
   <si>
@@ -438,13 +425,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>OKR複製</t>
-    <rPh sb="3" eb="5">
-      <t>フクセ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>OKR移動</t>
     <rPh sb="3" eb="5">
       <t>イド</t>
@@ -2441,6 +2421,21 @@
     </rPh>
     <rPh sb="7" eb="9">
       <t>ヘンコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/okrs/{slug}/clone.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OKRコピー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OKRのコピー・移動</t>
+    <rPh sb="8" eb="10">
+      <t>イド</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3287,7 +3282,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>13</v>
@@ -3968,49 +3963,49 @@
     </row>
     <row r="3" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -4039,7 +4034,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D5" s="5">
         <f>IF(B5=B4,IF(E5=E4,D4,D4+1),1)</f>
@@ -4055,23 +4050,23 @@
         <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O5" s="37" t="s">
         <v>12</v>
@@ -4089,7 +4084,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D6" s="5">
         <f>IF(B6=B5,IF(E6=E5,D5,D5+1),1)</f>
@@ -4105,23 +4100,23 @@
         <v>16</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="N6" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O6" s="37" t="s">
         <v>12</v>
@@ -4138,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D7" s="5">
         <f>IF(B7=B5,IF(E7=E5,D5,D5+1),1)</f>
@@ -4154,23 +4149,23 @@
         <v>16</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="N7" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O7" s="37" t="s">
         <v>12</v>
@@ -4206,20 +4201,20 @@
         <v>15</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="N8" s="31" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O8" s="37" t="s">
         <v>12</v>
@@ -4236,7 +4231,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" ref="D9:D92" si="2">IF(B9=B8,IF(E9=E8,D8,D8+1),1)</f>
@@ -4252,23 +4247,23 @@
         <v>16</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="K9" s="6" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="N9" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O9" s="37" t="s">
         <v>12</v>
@@ -4285,7 +4280,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" ref="D10" si="4">IF(B10=B9,IF(E10=E9,D9,D9+1),1)</f>
@@ -4302,23 +4297,23 @@
         <v>16</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O10" s="37" t="s">
         <v>12</v>
@@ -4335,14 +4330,14 @@
         <v>4</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11" s="5">
         <f>IF(B11=B9,IF(E11=E9,D9,D9+1),1)</f>
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="5">
         <v>1</v>
@@ -4351,23 +4346,23 @@
         <v>16</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O11" s="37" t="s">
         <v>12</v>
@@ -4384,14 +4379,14 @@
         <v>4</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="5"/>
@@ -4401,23 +4396,23 @@
         <v>5</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O12" s="37" t="s">
         <v>12</v>
@@ -4434,7 +4429,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="2"/>
@@ -4450,23 +4445,23 @@
         <v>5</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O13" s="37" t="s">
         <v>12</v>
@@ -4483,7 +4478,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="2"/>
@@ -4499,23 +4494,23 @@
         <v>5</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O14" s="37" t="s">
         <v>12</v>
@@ -4532,7 +4527,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="2"/>
@@ -4548,23 +4543,23 @@
         <v>5</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="O15" s="37" t="s">
         <v>12</v>
@@ -4581,7 +4576,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="2"/>
@@ -4598,23 +4593,23 @@
         <v>5</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O16" s="37" t="s">
         <v>12</v>
@@ -4631,7 +4626,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="2"/>
@@ -4651,20 +4646,20 @@
         <v>34</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O17" s="37" t="s">
         <v>12</v>
@@ -4681,7 +4676,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="2"/>
@@ -4695,28 +4690,30 @@
         <v>4</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>35</v>
+        <v>464</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>69</v>
+        <v>463</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>54</v>
+        <v>462</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="N18" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="O18" s="37"/>
+        <v>280</v>
+      </c>
+      <c r="O18" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
@@ -4728,7 +4725,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="2"/>
@@ -4742,26 +4739,26 @@
         <v>5</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>35</v>
+        <v>464</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N19" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O19" s="37"/>
     </row>
@@ -4775,7 +4772,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="2"/>
@@ -4789,26 +4786,26 @@
         <v>6</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N20" s="33" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O20" s="37" t="s">
         <v>12</v>
@@ -4825,14 +4822,14 @@
         <v>5</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="5"/>
@@ -4842,23 +4839,23 @@
         <v>3</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L21" s="6"/>
       <c r="M21" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O21" s="37" t="s">
         <v>12</v>
@@ -4875,40 +4872,40 @@
         <v>5</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="N22" s="33" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O22" s="37" t="s">
         <v>12</v>
@@ -4925,40 +4922,40 @@
         <v>5</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="N23" s="33" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O23" s="37" t="s">
         <v>12</v>
@@ -4975,40 +4972,40 @@
         <v>5</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N24" s="33" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O24" s="37" t="s">
         <v>12</v>
@@ -5025,40 +5022,40 @@
         <v>5</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D25" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F25" s="17">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="L25" s="17"/>
       <c r="M25" s="17" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O25" s="18" t="s">
         <v>12</v>
@@ -5075,40 +5072,40 @@
         <v>5</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" ref="D26" si="7">IF(B26=B25,IF(E26=E25,D25,D25+1),1)</f>
         <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="L26" s="6"/>
       <c r="M26" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="N26" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O26" s="37" t="s">
         <v>12</v>
@@ -5125,40 +5122,40 @@
         <v>5</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" ref="D27" si="9">IF(B27=B26,IF(E27=E26,D26,D26+1),1)</f>
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="N27" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O27" s="37" t="s">
         <v>12</v>
@@ -5175,40 +5172,40 @@
         <v>5</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28" s="5">
         <f>IF(B28=B25,IF(E28=E25,D25,D25+1),1)</f>
         <v>1</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O28" s="37" t="s">
         <v>12</v>
@@ -5225,40 +5222,40 @@
         <v>5</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D29" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="N29" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O29" s="37" t="s">
         <v>12</v>
@@ -5275,40 +5272,40 @@
         <v>5</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L30" s="6"/>
       <c r="M30" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="N30" s="33" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O30" s="37" t="s">
         <v>12</v>
@@ -5325,39 +5322,39 @@
         <v>6</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D31" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F31" s="17">
         <v>1</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H31" s="17" t="s">
         <v>30</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="L31" s="17"/>
       <c r="M31" s="17" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="N31" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O31" s="18" t="s">
         <v>12</v>
@@ -5374,14 +5371,14 @@
         <v>6</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D32" s="5">
         <f t="shared" ref="D32" si="11">IF(B32=B31,IF(E32=E31,D31,D31+1),1)</f>
         <v>1</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F32" s="5">
         <v>1</v>
@@ -5390,23 +5387,23 @@
         <v>5</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="N32" s="26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O32" s="37" t="s">
         <v>12</v>
@@ -5423,39 +5420,39 @@
         <v>6</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D33" s="17">
         <f t="shared" ref="D33:D39" si="13">IF(B33=B31,IF(E33=E31,D31,D31+1),1)</f>
         <v>2</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F33" s="17">
         <v>1</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>32</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O33" s="18" t="s">
         <v>12</v>
@@ -5472,14 +5469,14 @@
         <v>6</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D34" s="5">
         <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F34" s="5">
         <v>1</v>
@@ -5488,23 +5485,23 @@
         <v>5</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="N34" s="26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O34" s="37" t="s">
         <v>12</v>
@@ -5521,7 +5518,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D35" s="17">
         <f t="shared" si="13"/>
@@ -5534,26 +5531,26 @@
         <v>1</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>33</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L35" s="17"/>
       <c r="M35" s="17" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="N35" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O35" s="18" t="s">
         <v>12</v>
@@ -5570,7 +5567,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D36" s="5">
         <f t="shared" si="13"/>
@@ -5586,23 +5583,23 @@
         <v>5</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="L36" s="6"/>
       <c r="M36" s="5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="N36" s="26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O36" s="37" t="s">
         <v>12</v>
@@ -5619,39 +5616,39 @@
         <v>6</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D37" s="17">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F37" s="17">
         <v>1</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="K37" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L37" s="17"/>
       <c r="M37" s="17" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="N37" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O37" s="18" t="s">
         <v>12</v>
@@ -5668,14 +5665,14 @@
         <v>6</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D38" s="5">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="F38" s="5">
         <v>1</v>
@@ -5684,23 +5681,23 @@
         <v>5</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="L38" s="6"/>
       <c r="M38" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="N38" s="26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="O38" s="37" t="s">
         <v>12</v>
@@ -5733,23 +5730,23 @@
         <v>5</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N39" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O39" s="37" t="s">
         <v>12</v>
@@ -5783,23 +5780,23 @@
         <v>5</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L40" s="6"/>
       <c r="M40" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="N40" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O40" s="37" t="s">
         <v>12</v>
@@ -5823,7 +5820,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F41" s="5">
         <v>1</v>
@@ -5832,23 +5829,23 @@
         <v>5</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L41" s="6"/>
       <c r="M41" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="N41" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O41" s="37" t="s">
         <v>12</v>
@@ -5872,7 +5869,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F42" s="5">
         <f>F41+1</f>
@@ -5882,23 +5879,23 @@
         <v>5</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="N42" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O42" s="37" t="s">
         <v>12</v>
@@ -5922,7 +5919,7 @@
         <v>3</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F43" s="5">
         <v>1</v>
@@ -5931,23 +5928,23 @@
         <v>5</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L43" s="6"/>
       <c r="M43" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N43" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O43" s="37" t="s">
         <v>12</v>
@@ -5971,7 +5968,7 @@
         <v>3</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F44" s="5">
         <f>F43+1</f>
@@ -5981,23 +5978,23 @@
         <v>5</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="L44" s="6"/>
       <c r="M44" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N44" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O44" s="37" t="s">
         <v>12</v>
@@ -6021,7 +6018,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F45" s="5">
         <f>F44+1</f>
@@ -6031,23 +6028,23 @@
         <v>5</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L45" s="6"/>
       <c r="M45" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="N45" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O45" s="37" t="s">
         <v>12</v>
@@ -6071,7 +6068,7 @@
         <v>3</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F46" s="5">
         <f>F45+1</f>
@@ -6081,23 +6078,23 @@
         <v>5</v>
       </c>
       <c r="H46" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K46" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>390</v>
       </c>
       <c r="L46" s="6"/>
       <c r="M46" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="N46" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O46" s="37" t="s">
         <v>12</v>
@@ -6121,7 +6118,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F47" s="5">
         <f>F46+1</f>
@@ -6131,23 +6128,23 @@
         <v>5</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="L47" s="6"/>
       <c r="M47" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="N47" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O47" s="37" t="s">
         <v>12</v>
@@ -6164,7 +6161,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D48" s="5">
         <f>IF(B48=B44,IF(E48=E44,D44,D44+1),1)</f>
@@ -6180,23 +6177,23 @@
         <v>5</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L48" s="6"/>
       <c r="M48" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N48" s="29" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O48" s="37" t="s">
         <v>12</v>
@@ -6213,7 +6210,7 @@
         <v>8</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D49" s="5">
         <f t="shared" si="2"/>
@@ -6230,26 +6227,26 @@
         <v>5</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L49" s="6"/>
       <c r="M49" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N49" s="45" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O49" s="37" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P49" s="42"/>
     </row>
@@ -6263,43 +6260,43 @@
         <v>8</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D50" s="17">
         <f>IF(B50=B49,IF(E50=E49,D49,D49+1),1)</f>
         <v>1</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F50" s="17">
         <f>F49+1</f>
         <v>3</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L50" s="17"/>
       <c r="M50" s="17" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="N50" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O50" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P50" s="42"/>
     </row>
@@ -6313,7 +6310,7 @@
         <v>8</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D51" s="5">
         <f>IF(B51=B50,IF(E51=E50,D50,D50+1),1)</f>
@@ -6327,29 +6324,29 @@
         <v>4</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="N51" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O51" s="37" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P51" s="42"/>
     </row>
@@ -6363,7 +6360,7 @@
         <v>8</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D52" s="5">
         <f>IF(B52=B50,IF(E52=E50,D50,D50+1),1)</f>
@@ -6377,26 +6374,26 @@
         <v>5</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L52" s="6"/>
       <c r="M52" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N52" s="28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O52" s="37" t="s">
         <v>12</v>
@@ -6413,7 +6410,7 @@
         <v>8</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D53" s="5">
         <f t="shared" si="2"/>
@@ -6427,29 +6424,29 @@
         <v>6</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L53" s="6"/>
       <c r="M53" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="N53" s="28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O53" s="37" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P53" s="42"/>
     </row>
@@ -6463,7 +6460,7 @@
         <v>8</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D54" s="5">
         <f t="shared" si="2"/>
@@ -6479,23 +6476,23 @@
         <v>5</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L54" s="6"/>
       <c r="M54" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N54" s="28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O54" s="37" t="s">
         <v>12</v>
@@ -6512,7 +6509,7 @@
         <v>8</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D55" s="5">
         <f t="shared" si="2"/>
@@ -6529,23 +6526,23 @@
         <v>5</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L55" s="6"/>
       <c r="M55" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N55" s="29" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O55" s="37" t="s">
         <v>12</v>
@@ -6562,40 +6559,40 @@
         <v>8</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D56" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F56" s="17">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J56" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="L56" s="17"/>
       <c r="M56" s="17" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="N56" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O56" s="18" t="s">
         <v>12</v>
@@ -6612,40 +6609,40 @@
         <v>8</v>
       </c>
       <c r="C57" s="39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D57" s="5">
         <f t="shared" ref="D57" si="21">IF(B57=B56,IF(E57=E56,D56,D56+1),1)</f>
         <v>2</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F57" s="5">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G57" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H57" s="39" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="I57" s="39" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="J57" s="39" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K57" s="39" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="L57" s="39"/>
       <c r="M57" s="39" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="N57" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O57" s="37" t="s">
         <v>12</v>
@@ -6662,7 +6659,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D58" s="5">
         <f>IF(B58=B56,IF(E58=E56,D56,D56+1),1)</f>
@@ -6676,26 +6673,26 @@
         <v>5</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L58" s="6"/>
       <c r="M58" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N58" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O58" s="37" t="s">
         <v>12</v>
@@ -6712,7 +6709,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D59" s="5">
         <f t="shared" si="2"/>
@@ -6726,26 +6723,26 @@
         <v>6</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="L59" s="6"/>
       <c r="M59" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N59" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O59" s="37" t="s">
         <v>12</v>
@@ -6762,40 +6759,40 @@
         <v>8</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D60" s="17">
         <f>IF(B60=B64,IF(E60=E64,D64,D64+1),1)</f>
         <v>2</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F60" s="17">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J60" s="17" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L60" s="17"/>
       <c r="M60" s="17" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="N60" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O60" s="18" t="s">
         <v>12</v>
@@ -6812,40 +6809,40 @@
         <v>8</v>
       </c>
       <c r="C61" s="39" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D61" s="5">
         <f t="shared" ref="D61" si="23">IF(B61=B60,IF(E61=E60,D60,D60+1),1)</f>
         <v>2</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F61" s="5">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G61" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="L61" s="6"/>
       <c r="M61" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="N61" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O61" s="37" t="s">
         <v>12</v>
@@ -6862,40 +6859,40 @@
         <v>8</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D62" s="17">
         <f>IF(B62=B59,IF(E62=E59,D59,D59+1),1)</f>
         <v>2</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F62" s="17">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K62" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L62" s="17"/>
       <c r="M62" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N62" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O62" s="18"/>
     </row>
@@ -6909,40 +6906,40 @@
         <v>8</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D63" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F63" s="17">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I63" s="17" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K63" s="17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L63" s="17"/>
       <c r="M63" s="17" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="N63" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O63" s="18"/>
     </row>
@@ -6956,7 +6953,7 @@
         <v>8</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D64" s="5">
         <f t="shared" si="2"/>
@@ -6970,26 +6967,26 @@
         <v>11</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L64" s="6"/>
       <c r="M64" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N64" s="29" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O64" s="37" t="s">
         <v>12</v>
@@ -7006,40 +7003,40 @@
         <v>8</v>
       </c>
       <c r="C65" s="39" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D65" s="5">
         <f>IF(B65=B61,IF(E65=E61,D61,D61+1),1)</f>
         <v>2</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F65" s="5">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="G65" s="39" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="L65" s="6"/>
       <c r="M65" s="5" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="N65" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O65" s="37" t="s">
         <v>12</v>
@@ -7056,7 +7053,7 @@
         <v>8</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D66" s="5">
         <f>IF(B66=B60,IF(E66=E60,D60,D60+1),1)</f>
@@ -7070,26 +7067,26 @@
         <v>13</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="L66" s="6"/>
       <c r="M66" s="5" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="N66" s="29" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O66" s="37" t="s">
         <v>12</v>
@@ -7122,23 +7119,23 @@
         <v>5</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J67" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L67" s="17"/>
       <c r="M67" s="17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N67" s="17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O67" s="18"/>
     </row>
@@ -7168,26 +7165,26 @@
         <v>5</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K68" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L68" s="6"/>
       <c r="M68" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N68" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O68" s="37" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P68" s="42"/>
     </row>
@@ -7218,23 +7215,23 @@
         <v>31</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L69" s="6"/>
       <c r="M69" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="N69" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O69" s="37" t="s">
         <v>12</v>
@@ -7258,7 +7255,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F70" s="5">
         <v>1</v>
@@ -7267,25 +7264,25 @@
         <v>5</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N70" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O70" s="37" t="s">
         <v>12</v>
@@ -7309,7 +7306,7 @@
         <v>1</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F71" s="39">
         <f t="shared" si="5"/>
@@ -7319,23 +7316,23 @@
         <v>5</v>
       </c>
       <c r="H71" s="39" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I71" s="39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J71" s="39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K71" s="39" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L71" s="39"/>
       <c r="M71" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N71" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O71" s="37" t="s">
         <v>12</v>
@@ -7359,35 +7356,35 @@
         <v>1</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F72" s="5">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H72" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I72" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="L72" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="M72" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="I72" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="K72" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="L72" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="M72" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="N72" s="45" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O72" s="37" t="s">
         <v>12</v>
@@ -7411,35 +7408,35 @@
         <v>1</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F73" s="5">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H73" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="L73" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="I73" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K73" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="L73" s="6" t="s">
-        <v>299</v>
-      </c>
       <c r="M73" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="N73" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O73" s="37" t="s">
         <v>12</v>
@@ -7463,35 +7460,35 @@
         <v>1</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F74" s="5">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="G74" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H74" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="I74" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="L74" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="M74" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="J74" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="K74" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="L74" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="M74" s="5" t="s">
-        <v>310</v>
-      </c>
       <c r="N74" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O74" s="37" t="s">
         <v>12</v>
@@ -7515,35 +7512,35 @@
         <v>1</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F75" s="5">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L75" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="N75" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O75" s="37" t="s">
         <v>12</v>
@@ -7573,26 +7570,26 @@
         <v>1</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="I76" s="17" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J76" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K76" s="17" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="L76" s="17"/>
       <c r="M76" s="17" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="N76" s="17" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O76" s="18"/>
     </row>
@@ -7620,26 +7617,26 @@
         <v>2</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L77" s="6"/>
       <c r="M77" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="N77" s="29" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O77" s="37" t="s">
         <v>12</v>
@@ -7673,23 +7670,23 @@
         <v>5</v>
       </c>
       <c r="H78" s="39" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I78" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J78" s="39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K78" s="39" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="L78" s="39"/>
       <c r="M78" s="39" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N78" s="32" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O78" s="37" t="s">
         <v>12</v>
@@ -7720,26 +7717,26 @@
         <v>4</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I79" s="17" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="J79" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K79" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L79" s="17"/>
       <c r="M79" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N79" s="17" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="O79" s="18"/>
     </row>
@@ -7769,25 +7766,25 @@
         <v>5</v>
       </c>
       <c r="H80" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I80" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="N80" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O80" s="37" t="s">
         <v>12</v>
@@ -7820,25 +7817,25 @@
         <v>5</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L81" s="6" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="M81" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N81" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O81" s="37" t="s">
         <v>12</v>
@@ -7869,28 +7866,28 @@
         <v>2</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L82" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M82" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N82" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O82" s="37" t="s">
         <v>12</v>
@@ -7921,28 +7918,28 @@
         <v>3</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L83" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M83" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N83" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O83" s="37" t="s">
         <v>12</v>
@@ -7973,28 +7970,28 @@
         <v>4</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="L84" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M84" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="N84" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O84" s="37" t="s">
         <v>12</v>
@@ -8025,28 +8022,28 @@
         <v>5</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="L85" s="39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N85" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O85" s="37" t="s">
         <v>12</v>
@@ -8070,7 +8067,7 @@
         <v>5</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F86" s="5">
         <v>1</v>
@@ -8079,25 +8076,25 @@
         <v>5</v>
       </c>
       <c r="H86" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="I86" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="I86" s="5" t="s">
+      <c r="J86" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K86" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="J86" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K86" s="6" t="s">
-        <v>446</v>
-      </c>
       <c r="L86" s="39" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="N86" s="22" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="O86" s="37" t="s">
         <v>12</v>
@@ -8121,7 +8118,7 @@
         <v>6</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F87" s="5">
         <v>1</v>
@@ -8130,23 +8127,23 @@
         <v>5</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L87" s="39"/>
       <c r="M87" s="5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="N87" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O87" s="37" t="s">
         <v>12</v>
@@ -8170,7 +8167,7 @@
         <v>6</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F88" s="5">
         <v>1</v>
@@ -8179,23 +8176,23 @@
         <v>5</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="L88" s="39"/>
       <c r="M88" s="5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="N88" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O88" s="37" t="s">
         <v>12</v>
@@ -8228,25 +8225,25 @@
         <v>5</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L89" s="6" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="M89" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="N89" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O89" s="37" t="s">
         <v>12</v>
@@ -8279,25 +8276,25 @@
         <v>5</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J90" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L90" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N90" s="41" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O90" s="37" t="s">
         <v>12</v>
@@ -8330,23 +8327,23 @@
         <v>5</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L91" s="6"/>
       <c r="M91" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N91" s="34" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="O91" s="37" t="s">
         <v>12</v>
@@ -8363,14 +8360,14 @@
         <v>12</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D92" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F92" s="5">
         <v>1</v>
@@ -8379,23 +8376,23 @@
         <v>5</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I92" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K92" s="6" t="s">
         <v>397</v>
-      </c>
-      <c r="J92" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K92" s="6" t="s">
-        <v>400</v>
       </c>
       <c r="L92" s="6"/>
       <c r="M92" s="5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="N92" s="46" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="O92" s="37" t="s">
         <v>12</v>
@@ -8412,14 +8409,14 @@
         <v>12</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D93" s="5">
         <f t="shared" ref="D93" si="37">IF(B93=B92,IF(E93=E92,D92,D92+1),1)</f>
         <v>1</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F93" s="5">
         <v>1</v>
@@ -8428,23 +8425,23 @@
         <v>5</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I93" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K93" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K93" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="L93" s="6"/>
       <c r="M93" s="5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="N93" s="46" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="O93" s="37" t="s">
         <v>12</v>
@@ -8461,14 +8458,14 @@
         <v>12</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D94" s="5">
         <f t="shared" ref="D94" si="39">IF(B94=B93,IF(E94=E93,D93,D93+1),1)</f>
         <v>1</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F94" s="5">
         <v>1</v>
@@ -8477,23 +8474,23 @@
         <v>5</v>
       </c>
       <c r="H94" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K94" s="6" t="s">
         <v>403</v>
-      </c>
-      <c r="I94" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="J94" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K94" s="6" t="s">
-        <v>406</v>
       </c>
       <c r="L94" s="6"/>
       <c r="M94" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="N94" s="46" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="O94" s="37" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Timeline - Added a user timeline feature.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/APIList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/APIList.xlsx
@@ -16,7 +16,7 @@
     <sheet name="API一覧" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">API一覧!$A$4:$N$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">API一覧!$A$4:$N$92</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="470">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -2437,6 +2437,29 @@
     <rPh sb="8" eb="10">
       <t>イド</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムライン取得（ユーザ）</t>
+    <rPh sb="6" eb="8">
+      <t>シュトk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AG0101</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/users/{slug}/posts.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>getUserPostsAction($slug)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3900,7 +3923,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q127"/>
+  <dimension ref="A1:Q128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -4027,7 +4050,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <f t="shared" ref="A5:A81" si="0">ROW()-4</f>
+        <f t="shared" ref="A5:A82" si="0">ROW()-4</f>
         <v>1</v>
       </c>
       <c r="B5" s="5">
@@ -4234,7 +4257,7 @@
         <v>87</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" ref="D9:D92" si="2">IF(B9=B8,IF(E9=E8,D8,D8+1),1)</f>
+        <f t="shared" ref="D9:D93" si="2">IF(B9=B8,IF(E9=E8,D8,D8+1),1)</f>
         <v>1</v>
       </c>
       <c r="E9" s="16" t="s">
@@ -4276,7 +4299,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="5">
-        <f t="shared" ref="B10:B91" si="3">IF(C10=C9,B9,B9+1)</f>
+        <f t="shared" ref="B10:B92" si="3">IF(C10=C9,B9,B9+1)</f>
         <v>3</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -4290,7 +4313,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" ref="F10:F79" si="5">F9+1</f>
+        <f t="shared" ref="F10:F80" si="5">F9+1</f>
         <v>2</v>
       </c>
       <c r="G10" s="16" t="s">
@@ -5416,14 +5439,14 @@
         <v>29</v>
       </c>
       <c r="B33" s="17">
-        <f t="shared" ref="B33:B39" si="12">IF(C33=C31,B31,B31+1)</f>
+        <f t="shared" ref="B33:B38" si="12">IF(C33=C31,B31,B31+1)</f>
         <v>6</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>416</v>
       </c>
       <c r="D33" s="17">
-        <f t="shared" ref="D33:D39" si="13">IF(B33=B31,IF(E33=E31,D31,D31+1),1)</f>
+        <f t="shared" ref="D33:D48" si="13">IF(B33=B31,IF(E33=E31,D31,D31+1),1)</f>
         <v>2</v>
       </c>
       <c r="E33" s="17" t="s">
@@ -5668,7 +5691,7 @@
         <v>74</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -5710,18 +5733,18 @@
         <v>35</v>
       </c>
       <c r="B39" s="5">
-        <f t="shared" si="12"/>
+        <f>IF(C39=C36,B36,B36+1)</f>
         <v>7</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>22</v>
+        <v>465</v>
       </c>
       <c r="F39" s="5">
         <v>1</v>
@@ -5730,20 +5753,20 @@
         <v>5</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>338</v>
+        <v>466</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>134</v>
+        <v>467</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>58</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>56</v>
+        <v>468</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="5" t="s">
-        <v>190</v>
+        <v>469</v>
       </c>
       <c r="N39" s="27" t="s">
         <v>223</v>
@@ -5759,41 +5782,40 @@
         <v>36</v>
       </c>
       <c r="B40" s="5">
-        <f>IF(C40=C39,B39,B39+1)</f>
+        <f>IF(C40=C37,B37,B37+1)</f>
         <v>7</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="5">
-        <f>IF(B40=B39,IF(E40=E39,D39,D39+1),1)</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F40" s="5">
-        <f>F39+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="L40" s="6"/>
       <c r="M40" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N40" s="27" t="s">
         <v>223</v>
@@ -5809,40 +5831,41 @@
         <v>37</v>
       </c>
       <c r="B41" s="5">
-        <f>IF(C41=C39,B39,B39+1)</f>
+        <f>IF(C41=C40,B40,B40+1)</f>
         <v>7</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="5">
-        <f>IF(B41=B39,IF(E41=E39,D39,D39+1),1)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>342</v>
+        <v>22</v>
       </c>
       <c r="F41" s="5">
-        <v>1</v>
+        <f>F40+1</f>
+        <v>2</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>345</v>
+        <v>135</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>340</v>
+        <v>102</v>
       </c>
       <c r="L41" s="6"/>
       <c r="M41" s="5" t="s">
-        <v>341</v>
+        <v>191</v>
       </c>
       <c r="N41" s="27" t="s">
         <v>223</v>
@@ -5858,41 +5881,40 @@
         <v>38</v>
       </c>
       <c r="B42" s="5">
-        <f>IF(C42=C41,B41,B41+1)</f>
+        <f>IF(C42=C40,B40,B40+1)</f>
         <v>7</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" ref="D42:D45" si="14">IF(B42=B40,IF(E42=E40,D40,D40+1),1)</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>342</v>
       </c>
       <c r="F42" s="5">
-        <f>F41+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="K42" s="6" t="s">
         <v>340</v>
       </c>
       <c r="L42" s="6"/>
       <c r="M42" s="5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="N42" s="27" t="s">
         <v>223</v>
@@ -5908,40 +5930,41 @@
         <v>39</v>
       </c>
       <c r="B43" s="5">
-        <f>IF(C43=C40,B40,B40+1)</f>
+        <f>IF(C43=C42,B42,B42+1)</f>
         <v>7</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F43" s="5">
-        <v>1</v>
+        <f>F42+1</f>
+        <v>2</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>91</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>103</v>
+        <v>340</v>
       </c>
       <c r="L43" s="6"/>
       <c r="M43" s="5" t="s">
-        <v>192</v>
+        <v>347</v>
       </c>
       <c r="N43" s="27" t="s">
         <v>223</v>
@@ -5957,41 +5980,40 @@
         <v>40</v>
       </c>
       <c r="B44" s="5">
-        <f>IF(C44=C43,B43,B43+1)</f>
+        <f>IF(C44=C41,B41,B41+1)</f>
         <v>7</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="14"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>348</v>
       </c>
       <c r="F44" s="5">
-        <f>F43+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>79</v>
+        <v>332</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J44" s="5" t="s">
         <v>91</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>283</v>
+        <v>103</v>
       </c>
       <c r="L44" s="6"/>
       <c r="M44" s="5" t="s">
-        <v>284</v>
+        <v>192</v>
       </c>
       <c r="N44" s="27" t="s">
         <v>223</v>
@@ -6007,41 +6029,41 @@
         <v>41</v>
       </c>
       <c r="B45" s="5">
-        <f t="shared" ref="B45" si="15">IF(C45=C44,B44,B44+1)</f>
+        <f>IF(C45=C44,B44,B44+1)</f>
         <v>7</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="5">
-        <f t="shared" si="14"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>348</v>
       </c>
       <c r="F45" s="5">
         <f>F44+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>282</v>
+        <v>79</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>104</v>
+        <v>283</v>
       </c>
       <c r="L45" s="6"/>
       <c r="M45" s="5" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="N45" s="27" t="s">
         <v>223</v>
@@ -6057,41 +6079,41 @@
         <v>42</v>
       </c>
       <c r="B46" s="5">
-        <f t="shared" ref="B46" si="16">IF(C46=C45,B45,B45+1)</f>
+        <f t="shared" ref="B46" si="14">IF(C46=C45,B45,B45+1)</f>
         <v>7</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" ref="D46" si="17">IF(B46=B44,IF(E46=E44,D44,D44+1),1)</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>348</v>
       </c>
       <c r="F46" s="5">
         <f>F45+1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>384</v>
+        <v>282</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>386</v>
+        <v>351</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>108</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>387</v>
+        <v>104</v>
       </c>
       <c r="L46" s="6"/>
       <c r="M46" s="5" t="s">
-        <v>388</v>
+        <v>281</v>
       </c>
       <c r="N46" s="27" t="s">
         <v>223</v>
@@ -6107,41 +6129,41 @@
         <v>43</v>
       </c>
       <c r="B47" s="5">
-        <f t="shared" ref="B47" si="18">IF(C47=C46,B46,B46+1)</f>
+        <f t="shared" ref="B47" si="15">IF(C47=C46,B46,B46+1)</f>
         <v>7</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" ref="D47" si="19">IF(B47=B45,IF(E47=E45,D45,D45+1),1)</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>348</v>
       </c>
       <c r="F47" s="5">
         <f>F46+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L47" s="6"/>
       <c r="M47" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="N47" s="27" t="s">
         <v>223</v>
@@ -6157,43 +6179,44 @@
         <v>44</v>
       </c>
       <c r="B48" s="5">
-        <f>IF(C48=C44,B44,B44+1)</f>
-        <v>8</v>
+        <f t="shared" ref="B48" si="16">IF(C48=C47,B47,B47+1)</f>
+        <v>7</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="D48" s="5">
-        <f>IF(B48=B44,IF(E48=E44,D44,D44+1),1)</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>21</v>
+        <v>348</v>
       </c>
       <c r="F48" s="5">
-        <v>1</v>
+        <f>F47+1</f>
+        <v>5</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>5</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>83</v>
+        <v>385</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>136</v>
+        <v>391</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>105</v>
+        <v>389</v>
       </c>
       <c r="L48" s="6"/>
       <c r="M48" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="N48" s="29" t="s">
-        <v>243</v>
+        <v>390</v>
+      </c>
+      <c r="N48" s="27" t="s">
+        <v>223</v>
       </c>
       <c r="O48" s="37" t="s">
         <v>12</v>
@@ -6206,7 +6229,7 @@
         <v>45</v>
       </c>
       <c r="B49" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C49=C45,B45,B45+1)</f>
         <v>8</v>
       </c>
       <c r="C49" s="15" t="s">
@@ -6220,132 +6243,131 @@
         <v>21</v>
       </c>
       <c r="F49" s="5">
+        <v>1</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L49" s="6"/>
+      <c r="M49" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="N49" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="O49" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P49" s="42"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B50" s="5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G49" s="16" t="s">
+      <c r="G50" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H50" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I50" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J50" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K49" s="6" t="s">
+      <c r="K50" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="L49" s="6"/>
-      <c r="M49" s="5" t="s">
+      <c r="L50" s="6"/>
+      <c r="M50" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="N49" s="45" t="s">
+      <c r="N50" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="O49" s="37" t="s">
+      <c r="O50" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="P49" s="42"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A50" s="17">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B50" s="17">
-        <f>IF(C50=C49,B49,B49+1)</f>
-        <v>8</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="D50" s="17">
-        <f>IF(B50=B49,IF(E50=E49,D49,D49+1),1)</f>
-        <v>1</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F50" s="17">
-        <f>F49+1</f>
-        <v>3</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I50" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J50" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="K50" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="L50" s="17"/>
-      <c r="M50" s="17" t="s">
-        <v>367</v>
-      </c>
-      <c r="N50" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="O50" s="18" t="s">
-        <v>266</v>
-      </c>
       <c r="P50" s="42"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="5">
+      <c r="A51" s="17">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="17">
         <f>IF(C51=C50,B50,B50+1)</f>
         <v>8</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D51" s="5">
+      <c r="C51" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D51" s="17">
         <f>IF(B51=B50,IF(E51=E50,D50,D50+1),1)</f>
         <v>1</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="5">
+      <c r="E51" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" s="17">
         <f>F50+1</f>
-        <v>4</v>
-      </c>
-      <c r="G51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H51" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K51" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="L51" s="6"/>
-      <c r="M51" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="N51" s="32" t="s">
+      <c r="H51" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I51" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="J51" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="N51" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="O51" s="37" t="s">
+      <c r="O51" s="18" t="s">
         <v>266</v>
       </c>
       <c r="P51" s="42"/>
@@ -6356,14 +6378,14 @@
         <v>48</v>
       </c>
       <c r="B52" s="5">
-        <f>IF(C52=C50,B50,B50+1)</f>
+        <f>IF(C52=C51,B51,B51+1)</f>
         <v>8</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>78</v>
       </c>
       <c r="D52" s="5">
-        <f>IF(B52=B50,IF(E52=E50,D50,D50+1),1)</f>
+        <f>IF(B52=B51,IF(E52=E51,D51,D51+1),1)</f>
         <v>1</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -6371,32 +6393,32 @@
       </c>
       <c r="F52" s="5">
         <f>F51+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>85</v>
+        <v>373</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>107</v>
+        <v>374</v>
       </c>
       <c r="L52" s="6"/>
       <c r="M52" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="N52" s="28" t="s">
-        <v>225</v>
+        <v>375</v>
+      </c>
+      <c r="N52" s="32" t="s">
+        <v>274</v>
       </c>
       <c r="O52" s="37" t="s">
-        <v>12</v>
+        <v>266</v>
       </c>
       <c r="P52" s="42"/>
     </row>
@@ -6406,47 +6428,47 @@
         <v>49</v>
       </c>
       <c r="B53" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C53=C51,B51,B51+1)</f>
         <v>8</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>78</v>
       </c>
       <c r="D53" s="5">
-        <f t="shared" si="2"/>
+        <f>IF(B53=B51,IF(E53=E51,D51,D51+1),1)</f>
         <v>1</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F53" s="5">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f>F52+1</f>
+        <v>5</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>317</v>
+        <v>81</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>366</v>
+        <v>139</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="L53" s="6"/>
       <c r="M53" s="5" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="N53" s="28" t="s">
         <v>225</v>
       </c>
       <c r="O53" s="37" t="s">
-        <v>266</v>
+        <v>12</v>
       </c>
       <c r="P53" s="42"/>
     </row>
@@ -6464,38 +6486,39 @@
       </c>
       <c r="D54" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F54" s="5">
-        <v>1</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>317</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>140</v>
+        <v>366</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="L54" s="6"/>
       <c r="M54" s="5" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="N54" s="28" t="s">
         <v>225</v>
       </c>
       <c r="O54" s="37" t="s">
-        <v>12</v>
+        <v>266</v>
       </c>
       <c r="P54" s="42"/>
     </row>
@@ -6519,674 +6542,674 @@
         <v>22</v>
       </c>
       <c r="F55" s="5">
+        <v>1</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L55" s="6"/>
+      <c r="M55" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="N55" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="O55" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P55" s="42"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56" s="5">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B56" s="5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G55" s="16" t="s">
+      <c r="G56" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H56" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="I56" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J55" s="5" t="s">
+      <c r="J56" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K55" s="6" t="s">
+      <c r="K56" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L55" s="6"/>
-      <c r="M55" s="5" t="s">
+      <c r="L56" s="6"/>
+      <c r="M56" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="N55" s="29" t="s">
+      <c r="N56" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="O55" s="37" t="s">
+      <c r="O56" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P55" s="42"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A56" s="17">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B56" s="17">
+      <c r="P56" s="42"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A57" s="17">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B57" s="17">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C57" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D57" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E57" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F57" s="17">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="G57" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="H56" s="17" t="s">
+      <c r="H57" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="I56" s="17" t="s">
+      <c r="I57" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="J56" s="17" t="s">
+      <c r="J57" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="K56" s="17" t="s">
+      <c r="K57" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17" t="s">
+      <c r="L57" s="17"/>
+      <c r="M57" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="N56" s="17" t="s">
+      <c r="N57" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="O56" s="18" t="s">
+      <c r="O57" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P56" s="42"/>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A57" s="39">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B57" s="5">
-        <f t="shared" ref="B57" si="20">IF(C57=C56,B56,B56+1)</f>
+      <c r="P57" s="42"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A58" s="39">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B58" s="5">
+        <f t="shared" ref="B58" si="17">IF(C58=C57,B57,B57+1)</f>
         <v>8</v>
       </c>
-      <c r="C57" s="39" t="s">
+      <c r="C58" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="5">
-        <f t="shared" ref="D57" si="21">IF(B57=B56,IF(E57=E56,D56,D56+1),1)</f>
+      <c r="D58" s="5">
+        <f t="shared" ref="D58" si="18">IF(B58=B57,IF(E58=E57,D57,D57+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E57" s="39" t="s">
+      <c r="E58" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F58" s="5">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="G57" s="39" t="s">
+      <c r="G58" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="H57" s="39" t="s">
+      <c r="H58" s="39" t="s">
         <v>368</v>
       </c>
-      <c r="I57" s="39" t="s">
+      <c r="I58" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="J57" s="39" t="s">
+      <c r="J58" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="K57" s="39" t="s">
+      <c r="K58" s="39" t="s">
         <v>377</v>
       </c>
-      <c r="L57" s="39"/>
-      <c r="M57" s="39" t="s">
+      <c r="L58" s="39"/>
+      <c r="M58" s="39" t="s">
         <v>447</v>
       </c>
-      <c r="N57" s="32" t="s">
+      <c r="N58" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="O57" s="37" t="s">
+      <c r="O58" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P57" s="42"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A58" s="5">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B58" s="5">
-        <f>IF(C58=C56,B56,B56+1)</f>
+      <c r="P58" s="42"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A59" s="5">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B59" s="5">
+        <f>IF(C59=C57,B57,B57+1)</f>
         <v>8</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C59" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D58" s="5">
-        <f>IF(B58=B56,IF(E58=E56,D56,D56+1),1)</f>
+      <c r="D59" s="5">
+        <f>IF(B59=B57,IF(E59=E57,D57,D57+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F59" s="5">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="G58" s="5" t="s">
+      <c r="G59" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H59" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="I59" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="J58" s="5" t="s">
+      <c r="J59" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K58" s="6" t="s">
+      <c r="K59" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="L58" s="6"/>
-      <c r="M58" s="5" t="s">
+      <c r="L59" s="6"/>
+      <c r="M59" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="N58" s="30" t="s">
+      <c r="N59" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="O58" s="37" t="s">
+      <c r="O59" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P58" s="42"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A59" s="5">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B59" s="5">
+      <c r="P59" s="42"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60" s="5">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B60" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C60" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="5">
+      <c r="D60" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F59" s="5">
+      <c r="F60" s="5">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="G59" s="5" t="s">
+      <c r="G60" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H60" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I60" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="J59" s="5" t="s">
+      <c r="J60" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="K59" s="6" t="s">
+      <c r="K60" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="L59" s="6"/>
-      <c r="M59" s="5" t="s">
+      <c r="L60" s="6"/>
+      <c r="M60" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="N59" s="30" t="s">
+      <c r="N60" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="O59" s="37" t="s">
+      <c r="O60" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P59" s="42"/>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A60" s="17">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B60" s="17">
-        <f>IF(C60=C64,B64,B64+1)</f>
+      <c r="P60" s="42"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61" s="17">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B61" s="17">
+        <f>IF(C61=C65,B65,B65+1)</f>
         <v>8</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C61" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="17">
-        <f>IF(B60=B64,IF(E60=E64,D64,D64+1),1)</f>
+      <c r="D61" s="17">
+        <f>IF(B61=B65,IF(E61=E65,D65,D65+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E61" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F60" s="17">
+      <c r="F61" s="17">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="G60" s="17" t="s">
+      <c r="G61" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H60" s="17" t="s">
+      <c r="H61" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="I60" s="17" t="s">
+      <c r="I61" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="J60" s="17" t="s">
+      <c r="J61" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="K60" s="17" t="s">
+      <c r="K61" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17" t="s">
+      <c r="L61" s="17"/>
+      <c r="M61" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="N60" s="17" t="s">
+      <c r="N61" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="O60" s="18" t="s">
+      <c r="O61" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="P60" s="42"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="39">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B61" s="5">
-        <f t="shared" ref="B61" si="22">IF(C61=C60,B60,B60+1)</f>
+      <c r="P61" s="42"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62" s="39">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B62" s="5">
+        <f t="shared" ref="B62" si="19">IF(C62=C61,B61,B61+1)</f>
         <v>8</v>
       </c>
-      <c r="C61" s="39" t="s">
+      <c r="C62" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="D61" s="5">
-        <f t="shared" ref="D61" si="23">IF(B61=B60,IF(E61=E60,D60,D60+1),1)</f>
+      <c r="D62" s="5">
+        <f t="shared" ref="D62" si="20">IF(B62=B61,IF(E62=E61,D61,D61+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E61" s="39" t="s">
+      <c r="E62" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F61" s="5">
+      <c r="F62" s="5">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="G61" s="39" t="s">
+      <c r="G62" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H62" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I62" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="J61" s="5" t="s">
+      <c r="J62" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K61" s="6" t="s">
+      <c r="K62" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="L61" s="6"/>
-      <c r="M61" s="5" t="s">
+      <c r="L62" s="6"/>
+      <c r="M62" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="N61" s="32" t="s">
+      <c r="N62" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="O61" s="37" t="s">
+      <c r="O62" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P61" s="42"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A62" s="17">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B62" s="17">
-        <f>IF(C62=C59,B59,B59+1)</f>
+      <c r="P62" s="42"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63" s="17">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B63" s="17">
+        <f>IF(C63=C60,B60,B60+1)</f>
         <v>8</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C63" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="D62" s="17">
-        <f>IF(B62=B59,IF(E62=E59,D59,D59+1),1)</f>
+      <c r="D63" s="17">
+        <f>IF(B63=B60,IF(E63=E60,D60,D60+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E63" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F62" s="17">
+      <c r="F63" s="17">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="G63" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H62" s="17" t="s">
+      <c r="H63" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="I62" s="17" t="s">
+      <c r="I63" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J63" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="K62" s="17" t="s">
+      <c r="K63" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17" t="s">
+      <c r="L63" s="17"/>
+      <c r="M63" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="N62" s="17" t="s">
+      <c r="N63" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="O62" s="18"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A63" s="17">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B63" s="17">
+      <c r="O63" s="18"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A64" s="17">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B64" s="17">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C64" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D64" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E64" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F63" s="17">
+      <c r="F64" s="17">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="H63" s="17" t="s">
+      <c r="H64" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I63" s="17" t="s">
+      <c r="I64" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="J63" s="17" t="s">
+      <c r="J64" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K63" s="17" t="s">
+      <c r="K64" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17" t="s">
+      <c r="L64" s="17"/>
+      <c r="M64" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="N63" s="17" t="s">
+      <c r="N64" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="O63" s="18"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A64" s="5">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B64" s="5">
+      <c r="O64" s="18"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A65" s="5">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B65" s="5">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C65" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D65" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F65" s="5">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G64" s="5" t="s">
+      <c r="G65" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H65" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I65" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J65" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="K64" s="6" t="s">
+      <c r="K65" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="L64" s="6"/>
-      <c r="M64" s="5" t="s">
+      <c r="L65" s="6"/>
+      <c r="M65" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="N64" s="29" t="s">
+      <c r="N65" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="O64" s="37" t="s">
+      <c r="O65" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P64" s="42"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A65" s="39">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B65" s="5">
-        <f>IF(C65=C61,B61,B61+1)</f>
+      <c r="P65" s="42"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A66" s="39">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B66" s="5">
+        <f>IF(C66=C62,B62,B62+1)</f>
         <v>8</v>
       </c>
-      <c r="C65" s="39" t="s">
+      <c r="C66" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="D65" s="5">
-        <f>IF(B65=B61,IF(E65=E61,D61,D61+1),1)</f>
+      <c r="D66" s="5">
+        <f>IF(B66=B62,IF(E66=E62,D62,D62+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E65" s="39" t="s">
+      <c r="E66" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F65" s="5">
+      <c r="F66" s="5">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="G65" s="39" t="s">
+      <c r="G66" s="39" t="s">
         <v>270</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H66" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I66" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="J65" s="5" t="s">
+      <c r="J66" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K65" s="6" t="s">
+      <c r="K66" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="L65" s="6"/>
-      <c r="M65" s="5" t="s">
+      <c r="L66" s="6"/>
+      <c r="M66" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="N65" s="32" t="s">
+      <c r="N66" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="O65" s="37" t="s">
+      <c r="O66" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P65" s="42"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A66" s="5">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B66" s="5">
-        <f>IF(C66=C60,B60,B60+1)</f>
+      <c r="P66" s="42"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A67" s="5">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B67" s="5">
+        <f>IF(C67=C61,B61,B61+1)</f>
         <v>8</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C67" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D66" s="5">
-        <f>IF(B66=B60,IF(E66=E60,D60,D60+1),1)</f>
+      <c r="D67" s="5">
+        <f>IF(B67=B61,IF(E67=E61,D61,D61+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F66" s="5">
+      <c r="F67" s="5">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G67" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H67" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I67" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="J66" s="5" t="s">
+      <c r="J67" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="K66" s="6" t="s">
+      <c r="K67" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="L66" s="6"/>
-      <c r="M66" s="5" t="s">
+      <c r="L67" s="6"/>
+      <c r="M67" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="N66" s="29" t="s">
+      <c r="N67" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="O66" s="37" t="s">
+      <c r="O67" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P66" s="42"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A67" s="17">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B67" s="17">
+      <c r="P67" s="42"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A68" s="17">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B68" s="17">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C68" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D68" s="17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E67" s="18" t="s">
+      <c r="E68" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="17">
+      <c r="F68" s="17">
         <v>1</v>
       </c>
-      <c r="G67" s="18" t="s">
+      <c r="G68" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="17" t="s">
+      <c r="H68" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="I67" s="17" t="s">
+      <c r="I68" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="J68" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="K67" s="17" t="s">
+      <c r="K68" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="L67" s="17"/>
-      <c r="M67" s="17" t="s">
+      <c r="L68" s="17"/>
+      <c r="M68" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="N67" s="17" t="s">
+      <c r="N68" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="O67" s="18"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A68" s="5">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B68" s="5">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D68" s="5">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E68" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" s="5">
-        <v>1</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K68" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L68" s="6"/>
-      <c r="M68" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="N68" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="O68" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="P68" s="42"/>
+      <c r="O68" s="18"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
@@ -7208,33 +7231,32 @@
         <v>5</v>
       </c>
       <c r="F69" s="5">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>330</v>
+        <v>111</v>
       </c>
       <c r="L69" s="6"/>
       <c r="M69" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="N69" s="19" t="s">
-        <v>217</v>
+        <v>177</v>
+      </c>
+      <c r="N69" s="23" t="s">
+        <v>218</v>
       </c>
       <c r="O69" s="37" t="s">
-        <v>12</v>
+        <v>266</v>
       </c>
       <c r="P69" s="42"/>
     </row>
@@ -7245,44 +7267,43 @@
       </c>
       <c r="B70" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D70" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>61</v>
+      <c r="E70" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="F70" s="5">
-        <v>1</v>
-      </c>
-      <c r="G70" s="16" t="s">
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>251</v>
+        <v>86</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>91</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="L70" s="6" t="s">
-        <v>295</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="L70" s="6"/>
       <c r="M70" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="N70" s="34" t="s">
-        <v>245</v>
+        <v>331</v>
+      </c>
+      <c r="N70" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="O70" s="37" t="s">
         <v>12</v>
@@ -7290,101 +7311,100 @@
       <c r="P70" s="42"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A71" s="39">
+      <c r="A71" s="5">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B71" s="39">
+      <c r="B71" s="5">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C71" s="39" t="s">
+      <c r="C71" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D71" s="39">
+      <c r="D71" s="5">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E71" s="39" t="s">
+      <c r="E71" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F71" s="39">
+      <c r="F71" s="5">
+        <v>1</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="N71" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="O71" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P71" s="42"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" s="39">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B72" s="39">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="C72" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E72" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" s="39">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G71" s="40" t="s">
+      <c r="G72" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="H71" s="39" t="s">
+      <c r="H72" s="39" t="s">
         <v>324</v>
       </c>
-      <c r="I71" s="39" t="s">
+      <c r="I72" s="39" t="s">
         <v>227</v>
       </c>
-      <c r="J71" s="39" t="s">
+      <c r="J72" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="K71" s="39" t="s">
+      <c r="K72" s="39" t="s">
         <v>328</v>
       </c>
-      <c r="L71" s="39"/>
-      <c r="M71" s="39" t="s">
+      <c r="L72" s="39"/>
+      <c r="M72" s="39" t="s">
         <v>329</v>
       </c>
-      <c r="N71" s="32" t="s">
+      <c r="N72" s="32" t="s">
         <v>274</v>
-      </c>
-      <c r="O71" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P71" s="42"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A72" s="5">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="B72" s="5">
-        <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" s="5">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F72" s="5">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="K72" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="L72" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="M72" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="N72" s="45" t="s">
-        <v>221</v>
       </c>
       <c r="O72" s="37" t="s">
         <v>12</v>
@@ -7412,31 +7432,31 @@
       </c>
       <c r="F73" s="5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>293</v>
+        <v>226</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>91</v>
+        <v>228</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>289</v>
+        <v>152</v>
       </c>
       <c r="L73" s="6" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="M73" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="N73" s="34" t="s">
-        <v>245</v>
+        <v>229</v>
+      </c>
+      <c r="N73" s="45" t="s">
+        <v>221</v>
       </c>
       <c r="O73" s="37" t="s">
         <v>12</v>
@@ -7449,14 +7469,14 @@
         <v>70</v>
       </c>
       <c r="B74" s="5">
-        <f t="shared" ref="B74" si="24">IF(C74=C73,B73,B73+1)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="5">
-        <f t="shared" ref="D74" si="25">IF(B74=B73,IF(E74=E73,D73,D73+1),1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E74" s="5" t="s">
@@ -7464,28 +7484,28 @@
       </c>
       <c r="F74" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="L74" s="9" t="s">
-        <v>308</v>
+        <v>289</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>296</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="N74" s="34" t="s">
         <v>245</v>
@@ -7501,14 +7521,14 @@
         <v>71</v>
       </c>
       <c r="B75" s="5">
-        <f t="shared" ref="B75" si="26">IF(C75=C74,B74,B74+1)</f>
+        <f t="shared" ref="B75" si="21">IF(C75=C74,B74,B74+1)</f>
         <v>11</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="5">
-        <f t="shared" ref="D75" si="27">IF(B75=B74,IF(E75=E74,D74,D74+1),1)</f>
+        <f t="shared" ref="D75" si="22">IF(B75=B74,IF(E75=E74,D74,D74+1),1)</f>
         <v>1</v>
       </c>
       <c r="E75" s="5" t="s">
@@ -7516,28 +7536,28 @@
       </c>
       <c r="F75" s="5">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>302</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="L75" t="s">
+        <v>306</v>
+      </c>
+      <c r="L75" s="9" t="s">
         <v>308</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>450</v>
+        <v>307</v>
       </c>
       <c r="N75" s="34" t="s">
         <v>245</v>
@@ -7548,248 +7568,249 @@
       <c r="P75" s="42"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A76" s="17">
+      <c r="A76" s="5">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B76" s="17">
-        <f>IF(C76=C73,B73,B73+1)</f>
+      <c r="B76" s="5">
+        <f t="shared" ref="B76" si="23">IF(C76=C75,B75,B75+1)</f>
         <v>11</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="17">
-        <f>IF(B76=B73,IF(E76=E73,D73,D73+1),1)</f>
+      <c r="D76" s="5">
+        <f t="shared" ref="D76" si="24">IF(B76=B75,IF(E76=E75,D75,D75+1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F76" s="5">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="L76" t="s">
+        <v>308</v>
+      </c>
+      <c r="M76" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="N76" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="O76" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P76" s="42"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A77" s="17">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B77" s="17">
+        <f>IF(C77=C74,B74,B74+1)</f>
+        <v>11</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="17">
+        <f>IF(B77=B74,IF(E77=E74,D74,D74+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E76" s="17" t="s">
+      <c r="E77" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F76" s="17">
+      <c r="F77" s="17">
         <v>1</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="G77" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H76" s="17" t="s">
+      <c r="H77" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="I76" s="17" t="s">
+      <c r="I77" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="J76" s="17" t="s">
+      <c r="J77" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="K76" s="17" t="s">
+      <c r="K77" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="L76" s="17"/>
-      <c r="M76" s="17" t="s">
+      <c r="L77" s="17"/>
+      <c r="M77" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="N76" s="17" t="s">
+      <c r="N77" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="O76" s="18"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-      <c r="B77" s="5">
+      <c r="O77" s="18"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A78" s="5">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B78" s="5">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C78" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D78" s="5">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E77" s="6" t="s">
+      <c r="E78" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F78" s="5">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="G77" s="6" t="s">
+      <c r="G78" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="H78" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I78" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="J77" s="5" t="s">
+      <c r="J78" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K77" s="6" t="s">
+      <c r="K78" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="L77" s="6"/>
-      <c r="M77" s="5" t="s">
+      <c r="L78" s="6"/>
+      <c r="M78" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="N77" s="29" t="s">
+      <c r="N78" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="O77" s="37" t="s">
+      <c r="O78" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P77" s="42"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A78" s="39">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="B78" s="39">
+      <c r="P78" s="42"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A79" s="39">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B79" s="39">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="C78" s="39" t="s">
+      <c r="C79" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="39">
+      <c r="D79" s="39">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="E78" s="39" t="s">
+      <c r="E79" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F78" s="39">
+      <c r="F79" s="39">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="G78" s="40" t="s">
+      <c r="G79" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="H78" s="39" t="s">
+      <c r="H79" s="39" t="s">
         <v>325</v>
       </c>
-      <c r="I78" s="39" t="s">
+      <c r="I79" s="39" t="s">
         <v>313</v>
       </c>
-      <c r="J78" s="39" t="s">
+      <c r="J79" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="K78" s="39" t="s">
+      <c r="K79" s="39" t="s">
         <v>326</v>
       </c>
-      <c r="L78" s="39"/>
-      <c r="M78" s="39" t="s">
+      <c r="L79" s="39"/>
+      <c r="M79" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="N78" s="32" t="s">
+      <c r="N79" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="O78" s="37" t="s">
+      <c r="O79" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="P78" s="42"/>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A79" s="17">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="B79" s="17">
-        <f t="shared" ref="B79" si="28">IF(C79=C78,B78,B78+1)</f>
+      <c r="P79" s="42"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80" s="17">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B80" s="17">
+        <f t="shared" ref="B80" si="25">IF(C80=C79,B79,B79+1)</f>
         <v>11</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C80" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D79" s="17">
-        <f t="shared" ref="D79" si="29">IF(B79=B78,IF(E79=E78,D78,D78+1),1)</f>
+      <c r="D80" s="17">
+        <f t="shared" ref="D80" si="26">IF(B80=B79,IF(E80=E79,D79,D79+1),1)</f>
         <v>2</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E80" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="17">
+      <c r="F80" s="17">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="G79" s="17" t="s">
+      <c r="G80" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="H79" s="17" t="s">
+      <c r="H80" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I79" s="17" t="s">
+      <c r="I80" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="J79" s="17" t="s">
+      <c r="J80" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="K79" s="17" t="s">
+      <c r="K80" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="L79" s="17"/>
-      <c r="M79" s="17" t="s">
+      <c r="L80" s="17"/>
+      <c r="M80" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="N79" s="17" t="s">
+      <c r="N80" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="O79" s="18"/>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A80" s="5">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="B80" s="5">
-        <f>IF(C80=C78,B78,B78+1)</f>
-        <v>11</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D80" s="5">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F80" s="5">
-        <v>1</v>
-      </c>
-      <c r="G80" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K80" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L80" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="M80" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="N80" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="O80" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="P80" s="42"/>
+      <c r="O80" s="18"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
@@ -7817,13 +7838,13 @@
         <v>5</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>170</v>
+        <v>334</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>336</v>
+        <v>290</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="K81" s="6" t="s">
         <v>153</v>
@@ -7832,7 +7853,7 @@
         <v>297</v>
       </c>
       <c r="M81" s="5" t="s">
-        <v>180</v>
+        <v>335</v>
       </c>
       <c r="N81" s="25" t="s">
         <v>235</v>
@@ -7844,11 +7865,11 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
-        <f t="shared" ref="A82:A94" si="30">ROW()-4</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
       <c r="B82" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C82=C80,B80,B80+1)</f>
         <v>11</v>
       </c>
       <c r="C82" s="15" t="s">
@@ -7856,38 +7877,37 @@
       </c>
       <c r="D82" s="5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F82" s="5">
-        <f t="shared" ref="F82:F85" si="31">F81+1</f>
-        <v>2</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>46</v>
+        <v>1</v>
+      </c>
+      <c r="G82" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="H82" s="5" t="s">
-        <v>46</v>
+        <v>170</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>147</v>
+        <v>336</v>
       </c>
       <c r="J82" s="5" t="s">
         <v>98</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="L82" s="39" t="s">
-        <v>298</v>
+        <v>153</v>
+      </c>
+      <c r="L82" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="M82" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="N82" s="23" t="s">
-        <v>218</v>
+        <v>180</v>
+      </c>
+      <c r="N82" s="25" t="s">
+        <v>235</v>
       </c>
       <c r="O82" s="37" t="s">
         <v>12</v>
@@ -7896,7 +7916,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="A83:A95" si="27">ROW()-4</f>
         <v>79</v>
       </c>
       <c r="B83" s="5">
@@ -7914,29 +7934,29 @@
         <v>26</v>
       </c>
       <c r="F83" s="5">
-        <f t="shared" si="31"/>
-        <v>3</v>
+        <f t="shared" ref="F83:F86" si="28">F82+1</f>
+        <v>2</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I83" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="L83" s="39" t="s">
         <v>298</v>
       </c>
       <c r="M83" s="5" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="N83" s="23" t="s">
         <v>218</v>
@@ -7948,7 +7968,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>80</v>
       </c>
       <c r="B84" s="5">
@@ -7966,29 +7986,29 @@
         <v>26</v>
       </c>
       <c r="F84" s="5">
-        <f t="shared" si="31"/>
-        <v>4</v>
+        <f t="shared" si="28"/>
+        <v>3</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>323</v>
+        <v>47</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="L84" s="39" t="s">
         <v>298</v>
       </c>
       <c r="M84" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N84" s="23" t="s">
         <v>218</v>
@@ -8000,7 +8020,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>81</v>
       </c>
       <c r="B85" s="5">
@@ -8018,29 +8038,29 @@
         <v>26</v>
       </c>
       <c r="F85" s="5">
-        <f t="shared" si="31"/>
-        <v>5</v>
+        <f t="shared" si="28"/>
+        <v>4</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>48</v>
+        <v>323</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>279</v>
+        <v>189</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="L85" s="39" t="s">
         <v>298</v>
       </c>
       <c r="M85" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N85" s="23" t="s">
         <v>218</v>
@@ -8052,11 +8072,11 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>82</v>
       </c>
       <c r="B86" s="5">
-        <f t="shared" ref="B86" si="32">IF(C86=C85,B85,B85+1)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="C86" s="15" t="s">
@@ -8064,37 +8084,38 @@
       </c>
       <c r="D86" s="5">
         <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" s="5">
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
-      <c r="E86" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="F86" s="5">
-        <v>1</v>
-      </c>
-      <c r="G86" s="16" t="s">
-        <v>5</v>
+      <c r="G86" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>437</v>
+        <v>48</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>440</v>
+        <v>279</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>443</v>
+        <v>154</v>
       </c>
       <c r="L86" s="39" t="s">
-        <v>442</v>
+        <v>298</v>
       </c>
       <c r="M86" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="N86" s="22" t="s">
-        <v>441</v>
+        <v>176</v>
+      </c>
+      <c r="N86" s="23" t="s">
+        <v>218</v>
       </c>
       <c r="O86" s="37" t="s">
         <v>12</v>
@@ -8103,11 +8124,11 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>83</v>
       </c>
       <c r="B87" s="5">
-        <f t="shared" ref="B87" si="33">IF(C87=C86,B86,B86+1)</f>
+        <f t="shared" ref="B87" si="29">IF(C87=C86,B86,B86+1)</f>
         <v>11</v>
       </c>
       <c r="C87" s="15" t="s">
@@ -8115,10 +8136,10 @@
       </c>
       <c r="D87" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="F87" s="5">
         <v>1</v>
@@ -8127,23 +8148,25 @@
         <v>5</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>458</v>
+        <v>437</v>
       </c>
       <c r="I87" s="5" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>419</v>
+        <v>91</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="L87" s="39"/>
+        <v>443</v>
+      </c>
+      <c r="L87" s="39" t="s">
+        <v>442</v>
+      </c>
       <c r="M87" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="N87" s="34" t="s">
-        <v>245</v>
+        <v>444</v>
+      </c>
+      <c r="N87" s="22" t="s">
+        <v>441</v>
       </c>
       <c r="O87" s="37" t="s">
         <v>12</v>
@@ -8152,11 +8175,11 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>84</v>
       </c>
       <c r="B88" s="5">
-        <f t="shared" ref="B88" si="34">IF(C88=C87,B87,B87+1)</f>
+        <f t="shared" ref="B88" si="30">IF(C88=C87,B87,B87+1)</f>
         <v>11</v>
       </c>
       <c r="C88" s="15" t="s">
@@ -8176,20 +8199,20 @@
         <v>5</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I88" s="5" t="s">
-        <v>459</v>
+        <v>439</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>272</v>
+        <v>419</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L88" s="39"/>
       <c r="M88" s="5" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="N88" s="34" t="s">
         <v>245</v>
@@ -8201,11 +8224,11 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>85</v>
       </c>
       <c r="B89" s="5">
-        <f>IF(C89=C85,B85,B85+1)</f>
+        <f t="shared" ref="B89" si="31">IF(C89=C88,B88,B88+1)</f>
         <v>11</v>
       </c>
       <c r="C89" s="15" t="s">
@@ -8213,10 +8236,10 @@
       </c>
       <c r="D89" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>27</v>
+        <v>452</v>
       </c>
       <c r="F89" s="5">
         <v>1</v>
@@ -8225,25 +8248,23 @@
         <v>5</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>287</v>
+        <v>461</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>110</v>
+        <v>272</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="L89" s="6" t="s">
-        <v>299</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="L89" s="39"/>
       <c r="M89" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="N89" s="24" t="s">
-        <v>219</v>
+        <v>457</v>
+      </c>
+      <c r="N89" s="34" t="s">
+        <v>245</v>
       </c>
       <c r="O89" s="37" t="s">
         <v>12</v>
@@ -8252,11 +8273,11 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>86</v>
       </c>
       <c r="B90" s="5">
-        <f t="shared" si="3"/>
+        <f>IF(C90=C86,B86,B86+1)</f>
         <v>11</v>
       </c>
       <c r="C90" s="15" t="s">
@@ -8264,10 +8285,10 @@
       </c>
       <c r="D90" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F90" s="5">
         <v>1</v>
@@ -8276,25 +8297,25 @@
         <v>5</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>49</v>
+        <v>287</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>438</v>
+        <v>454</v>
       </c>
       <c r="J90" s="5" t="s">
         <v>110</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>157</v>
+        <v>337</v>
       </c>
       <c r="L90" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M90" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="N90" s="41" t="s">
-        <v>220</v>
+        <v>178</v>
+      </c>
+      <c r="N90" s="24" t="s">
+        <v>219</v>
       </c>
       <c r="O90" s="37" t="s">
         <v>12</v>
@@ -8303,7 +8324,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>87</v>
       </c>
       <c r="B91" s="5">
@@ -8315,10 +8336,10 @@
       </c>
       <c r="D91" s="5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F91" s="5">
         <v>1</v>
@@ -8327,23 +8348,25 @@
         <v>5</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>292</v>
+        <v>49</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="L91" s="6"/>
+        <v>157</v>
+      </c>
+      <c r="L91" s="6" t="s">
+        <v>300</v>
+      </c>
       <c r="M91" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="N91" s="34" t="s">
-        <v>245</v>
+        <v>179</v>
+      </c>
+      <c r="N91" s="41" t="s">
+        <v>220</v>
       </c>
       <c r="O91" s="37" t="s">
         <v>12</v>
@@ -8352,22 +8375,22 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>88</v>
       </c>
       <c r="B92" s="5">
-        <f t="shared" ref="B92" si="35">IF(C92=C91,B91,B91+1)</f>
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>11</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>393</v>
+        <v>20</v>
       </c>
       <c r="D92" s="5">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>392</v>
+        <v>29</v>
       </c>
       <c r="F92" s="5">
         <v>1</v>
@@ -8376,23 +8399,23 @@
         <v>5</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>396</v>
+        <v>292</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>394</v>
+        <v>453</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>397</v>
+        <v>158</v>
       </c>
       <c r="L92" s="6"/>
       <c r="M92" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="N92" s="46" t="s">
-        <v>395</v>
+        <v>213</v>
+      </c>
+      <c r="N92" s="34" t="s">
+        <v>245</v>
       </c>
       <c r="O92" s="37" t="s">
         <v>12</v>
@@ -8401,18 +8424,18 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>89</v>
       </c>
       <c r="B93" s="5">
-        <f t="shared" ref="B93" si="36">IF(C93=C92,B92,B92+1)</f>
+        <f t="shared" ref="B93" si="32">IF(C93=C92,B92,B92+1)</f>
         <v>12</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>393</v>
       </c>
       <c r="D93" s="5">
-        <f t="shared" ref="D93" si="37">IF(B93=B92,IF(E93=E92,D92,D92+1),1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E93" s="6" t="s">
@@ -8425,20 +8448,20 @@
         <v>5</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="J93" s="5" t="s">
         <v>91</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="L93" s="6"/>
       <c r="M93" s="5" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="N93" s="46" t="s">
         <v>395</v>
@@ -8450,18 +8473,18 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
-        <f t="shared" si="30"/>
+        <f t="shared" si="27"/>
         <v>90</v>
       </c>
       <c r="B94" s="5">
-        <f t="shared" ref="B94" si="38">IF(C94=C93,B93,B93+1)</f>
+        <f t="shared" ref="B94" si="33">IF(C94=C93,B93,B93+1)</f>
         <v>12</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>393</v>
       </c>
       <c r="D94" s="5">
-        <f t="shared" ref="D94" si="39">IF(B94=B93,IF(E94=E93,D93,D93+1),1)</f>
+        <f t="shared" ref="D94" si="34">IF(B94=B93,IF(E94=E93,D93,D93+1),1)</f>
         <v>1</v>
       </c>
       <c r="E94" s="6" t="s">
@@ -8474,20 +8497,20 @@
         <v>5</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J94" s="5" t="s">
         <v>91</v>
       </c>
       <c r="K94" s="6" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="L94" s="6"/>
       <c r="M94" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N94" s="46" t="s">
         <v>395</v>
@@ -8498,11 +8521,53 @@
       <c r="P94" s="42"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
+      <c r="A95" s="5">
+        <f t="shared" si="27"/>
+        <v>91</v>
+      </c>
+      <c r="B95" s="5">
+        <f t="shared" ref="B95" si="35">IF(C95=C94,B94,B94+1)</f>
+        <v>12</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="D95" s="5">
+        <f t="shared" ref="D95" si="36">IF(B95=B94,IF(E95=E94,D94,D94+1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="F95" s="5">
+        <v>1</v>
+      </c>
+      <c r="G95" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="L95" s="6"/>
+      <c r="M95" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="N95" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="O95" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P95" s="42"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B96" s="4"/>
@@ -8728,8 +8793,15 @@
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
     </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:N91"/>
+  <autoFilter ref="A4:N92"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Revised getNewOneOnOnes and Made hearing due date reminder email batch.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/APIList.xlsx
+++ b/skrum_docs/02_SpecificationDocs/APIList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="510">
   <si>
     <t>#</t>
     <phoneticPr fontId="1"/>
@@ -2650,6 +2650,30 @@
   </si>
   <si>
     <t>getUserDefaultdestinationsAction($slug)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サポート</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>目標一括登録CSVアップロード</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AS0101</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/csv/okrs.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>postCsvOkrsAction()</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -8115,7 +8139,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
-        <f t="shared" ref="A83:A103" si="27">ROW()-4</f>
+        <f t="shared" ref="A83:A104" si="27">ROW()-4</f>
         <v>79</v>
       </c>
       <c r="B83" s="5">
@@ -9161,11 +9185,53 @@
       <c r="P103" s="42"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
+      <c r="A104" s="5">
+        <f t="shared" si="27"/>
+        <v>100</v>
+      </c>
+      <c r="B104" s="5">
+        <f t="shared" ref="B104" si="42">IF(C104=C103,B103,B103+1)</f>
+        <v>14</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="D104" s="5">
+        <f t="shared" ref="D104" si="43">IF(B104=B103,IF(E104=E103,D103,D103+1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="F104" s="5">
+        <v>1</v>
+      </c>
+      <c r="G104" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K104" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="L104" s="39"/>
+      <c r="M104" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="N104" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="O104" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P104" s="42"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B105" s="4"/>

</xml_diff>